<commit_message>
Updates to mapping table, org profiles
</commit_message>
<xml_diff>
--- a/mapping/Mappings.xlsx
+++ b/mapping/Mappings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Lantana Consulting Group\CDC MITRE eICR - Documents\FHIR eCR\Mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{8D50DC6F-6599-479B-AE13-FD1E6FB28F4C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{738F156E-5B71-40BA-A4F0-D7168F4E9EEC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D0F7F4-E09F-40BA-953B-9C8364247CE0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" activeTab="1" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
   </bookViews>
   <sheets>
     <sheet name="RR" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="321">
   <si>
     <t>Date and time of eICR Receipt</t>
   </si>
@@ -265,9 +265,6 @@
     <t>Parent/ Guardian Name</t>
   </si>
   <si>
-    <t>Clinical Document/record target/patientRole/patient/guardian/guradianPerson/name</t>
-  </si>
-  <si>
     <t>PN</t>
   </si>
   <si>
@@ -541,9 +538,6 @@
     <t>FHIR</t>
   </si>
   <si>
-    <t>Communication.topic.extension</t>
-  </si>
-  <si>
     <t>Reportability Response/effectiveTime</t>
   </si>
   <si>
@@ -905,6 +899,102 @@
   </si>
   <si>
     <t>us-core-patient.extension:us-core-birthsex</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working on this </t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation(PlanDefinition).contentReference: rr-plandefinition.extension-rr-determination-of-reportability-reason</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.contentReference:rr-plandefinition.extension-rr-determination-of-reportability-rule</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.contentReference: rr-plandefinition.extension-rr-determination-of-reportability</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceEICRInformation.contentReference.identifier</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).context: eicr-encounter.id</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceEICRInformation.extension-rr-eicr-processing-status</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-location-relevance</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).action.documentation.extension-rr-external-resource-priority</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).action.documentation.url</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).action.documentation.display</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).action.documentation.extension-rr-external-resource-type</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).goal.address.coding.display</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).goal.address.coding.code</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).topic.display</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceReportabilityResponseSummary.contentString</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).identifier</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).timingDuration</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).subject.us-core-patient (Patient).gender</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).subject.us-core-patient (Patient).birthdate</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).subject.us-core-patient (Patient).us-core-ethnicity</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).subject.us-core-patient (Patient).us-core-race</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).subject.us-core-patient (Patient).identifier</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).subject.us-core-patient (Patient).name</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).subject.us-core-patient (Patient).communication.language</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload: sliceEICRInformation.extension-rr-manually-initiated-eicr</t>
+  </si>
+  <si>
+    <t>Clinical Document/record target/patientRole/patient/guardian/guardianPerson/name</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-responsible-agency.rr-responsible-agency (US Core Organization).telecom</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-responsible-agency.rr-responsible-agency (US Core Organization).address</t>
   </si>
 </sst>
 </file>
@@ -983,9 +1073,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -997,6 +1084,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1315,11 +1405,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2E64F1-05B1-4B7F-9A17-F737E551CA1E}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="77.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,27 +1418,32 @@
     <col min="2" max="2" width="33.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="77.140625" style="3"/>
     <col min="4" max="4" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="77.140625" style="3"/>
+    <col min="5" max="5" width="42.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="77.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1362,7 +1457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1375,11 +1470,11 @@
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+      <c r="E3" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1392,11 +1487,11 @@
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="E4" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1409,8 +1504,11 @@
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1423,8 +1521,11 @@
       <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1437,8 +1538,11 @@
       <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1451,8 +1555,11 @@
       <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1465,8 +1572,14 @@
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1479,8 +1592,14 @@
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1493,8 +1612,14 @@
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -1507,8 +1632,14 @@
       <c r="D12" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>35</v>
       </c>
@@ -1521,8 +1652,14 @@
       <c r="D13" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="E13" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
@@ -1535,8 +1672,14 @@
       <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -1549,8 +1692,11 @@
       <c r="D15" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1563,8 +1709,11 @@
       <c r="D16" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="48" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
@@ -1577,8 +1726,11 @@
       <c r="D17" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -1591,8 +1743,11 @@
       <c r="D18" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="E18" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
@@ -1606,7 +1761,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -1620,7 +1775,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -1634,7 +1789,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
@@ -1648,7 +1803,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>60</v>
       </c>
@@ -1662,7 +1817,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -1676,7 +1831,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>64</v>
       </c>
@@ -1690,7 +1845,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>66</v>
       </c>
@@ -1704,7 +1859,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>68</v>
       </c>
@@ -1717,8 +1872,11 @@
       <c r="D27" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="36" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>70</v>
       </c>
@@ -1731,8 +1889,11 @@
       <c r="D28" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>72</v>
       </c>
@@ -1746,7 +1907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -1760,7 +1921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>76</v>
       </c>
@@ -1768,453 +1929,501 @@
         <v>22</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="E40" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="D43" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D44" s="9"/>
+    </row>
+    <row r="45" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="C45" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="D45" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="9"/>
+    </row>
+    <row r="47" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" s="4" t="s">
+      <c r="C47" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D48" s="9"/>
+    </row>
+    <row r="49" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B47" s="4" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" s="9"/>
+    </row>
+    <row r="51" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B51" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B49" s="4" t="s">
+      <c r="C51" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="9"/>
+    </row>
+    <row r="53" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D49" s="4" t="s">
+      <c r="C53" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" s="9"/>
+    </row>
+    <row r="55" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="4"/>
-    </row>
-    <row r="53" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C55" s="2" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="9"/>
+    </row>
+    <row r="57" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="D56" s="4"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F59" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="E62" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C63" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E64" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="72" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="E65" s="4" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="66" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>34</v>
@@ -2222,13 +2431,13 @@
     </row>
     <row r="67" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>15</v>
@@ -2236,27 +2445,27 @@
     </row>
     <row r="68" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>52</v>
@@ -2264,13 +2473,13 @@
     </row>
     <row r="70" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>37</v>
@@ -2278,13 +2487,13 @@
     </row>
     <row r="71" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>34</v>
@@ -2292,13 +2501,13 @@
     </row>
     <row r="72" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>15</v>
@@ -2306,27 +2515,27 @@
     </row>
     <row r="73" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>52</v>
@@ -2334,13 +2543,13 @@
     </row>
     <row r="75" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>37</v>
@@ -2348,13 +2557,13 @@
     </row>
     <row r="76" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>34</v>
@@ -2362,13 +2571,13 @@
     </row>
     <row r="77" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>15</v>
@@ -2376,39 +2585,51 @@
     </row>
     <row r="78" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C79" s="5" t="s">
+      <c r="C79" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C80" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E79" s="3" t="s">
+      <c r="E80" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F80" s="3" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C80" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="D55:D56"/>
@@ -2418,18 +2639,6 @@
     <mergeCell ref="A53:A54"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D45:D46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2440,141 +2649,141 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1E071C-8572-48FD-94ED-9BC2BF0CD944}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.42578125" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.42578125" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -2583,10 +2792,10 @@
         <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -2595,10 +2804,10 @@
         <v>55</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -2607,10 +2816,10 @@
         <v>62</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -2619,27 +2828,27 @@
         <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.2">
@@ -2647,81 +2856,81 @@
         <v>50</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D16" s="7"/>
+        <v>196</v>
+      </c>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="24" x14ac:dyDescent="0.2">
@@ -2729,27 +2938,27 @@
         <v>76</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="24" x14ac:dyDescent="0.2">
@@ -2757,549 +2966,556 @@
         <v>74</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="D24" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="E27" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="B28" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="D28" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="D29" s="4"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>288</v>
+        <v>182</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B32" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="C32" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="D32" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
       <c r="D33" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D35" s="7"/>
+        <v>191</v>
+      </c>
+      <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>242</v>
-      </c>
       <c r="D40" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+      <c r="C43" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="D43" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C43" s="4" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="2" t="s">
+      <c r="C45" s="9" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="B45" s="4" t="s">
+      <c r="D45" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C45" s="4" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="2" t="s">
+      <c r="B47" s="9" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+      <c r="C47" s="9"/>
+      <c r="D47" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="C49" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>256</v>
-      </c>
       <c r="D49" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
       <c r="D50" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
+      <c r="C53" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="D53" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="9"/>
+      <c r="B54" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D54" s="9"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="4"/>
-      <c r="B54" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C54" s="2" t="s">
+      <c r="B55" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>266</v>
-      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
       <c r="D56" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="D57" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="36" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="D59" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>281</v>
       </c>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" ht="36" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" ht="36" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D65" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="C55:C56"/>
@@ -3309,18 +3525,11 @@
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="C47:C48"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="D53:D54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3328,6 +3537,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E2A70C0F482D004F81B909595C75DFA6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e14e4ad0a6f5f1a0ddcbf041a2a4a832">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="9ed5a28f-e285-4793-933e-f86572ea3e88" xmlns:ns3="6FDAA894-E433-443A-929C-6668B5175CA9" xmlns:ns4="a130c0bc-081d-4a7d-8c4b-0d956631a56e" xmlns:ns5="6fdaa894-e433-443a-929c-6668b5175ca9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f3fa50635c17e9cfabaeee8fe605afa8" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3532,15 +3750,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3555,6 +3764,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{211F509A-75D2-471F-BE44-DEEBD2FE04CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28D2A50F-394A-4741-95EF-7EE6194A4F57}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3572,14 +3789,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{211F509A-75D2-471F-BE44-DEEBD2FE04CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated names of extensions, mapping table, fixed random errors
</commit_message>
<xml_diff>
--- a/mapping/Mappings.xlsx
+++ b/mapping/Mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D0F7F4-E09F-40BA-953B-9C8364247CE0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62771155-8ECC-4F13-B75C-68F0D5EFFA8E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="334">
   <si>
     <t>Date and time of eICR Receipt</t>
   </si>
@@ -995,6 +995,45 @@
   </si>
   <si>
     <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-responsible-agency.rr-responsible-agency (US Core Organization).address</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-routing-entity.rr-routing-entity (US Core Organization).address</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-responsible-agency.rr-responsible-agency (US Core Organization).text</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-responsible-agency.rr-responsible-agency (US Core Organization).identifier</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-responsible-agency.rr-responsible-agency (US Core Organization).name</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-routing-entity.rr-routing-entity (US Core Organization).text</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-routing-entity.rr-routing-entity (US Core Organization).identifier</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-routing-entity.rr-routing-entity (US Core Organization).name</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-routing-entity.rr-routing-entity (US Core Organization).telecom</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-rules-authoring-agency.rr-rules-authoring-agency (US Core Organization).address</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-rules-authoring-agency.rr-rules-authoring-agency (US Core Organization).telecom</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-rules-authoring-agency.rr-rules-authoring-agency (US Core Organization).text</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-rules-authoring-agency.rr-rules-authoring-agency (US Core Organization).identifier</t>
+  </si>
+  <si>
+    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-rules-authoring-agency.rr-rules-authoring-agency (US Core Organization).name</t>
   </si>
 </sst>
 </file>
@@ -1406,10 +1445,10 @@
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomRight" activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="77.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2415,7 +2454,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="72" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>141</v>
       </c>
@@ -2428,8 +2467,11 @@
       <c r="D66" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="E66" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="72" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>143</v>
       </c>
@@ -2442,8 +2484,11 @@
       <c r="D67" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E67" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="72" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>145</v>
       </c>
@@ -2456,8 +2501,11 @@
       <c r="D68" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="E68" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="72" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>147</v>
       </c>
@@ -2470,8 +2518,11 @@
       <c r="D69" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="E69" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="72" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>149</v>
       </c>
@@ -2484,8 +2535,11 @@
       <c r="D70" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E70" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>151</v>
       </c>
@@ -2498,8 +2552,11 @@
       <c r="D71" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E71" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="72" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>153</v>
       </c>
@@ -2512,8 +2569,11 @@
       <c r="D72" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E72" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>155</v>
       </c>
@@ -2526,8 +2586,11 @@
       <c r="D73" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="E73" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="72" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>157</v>
       </c>
@@ -2540,8 +2603,11 @@
       <c r="D74" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E74" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="72" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>159</v>
       </c>
@@ -2554,8 +2620,11 @@
       <c r="D75" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E75" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>161</v>
       </c>
@@ -2568,8 +2637,11 @@
       <c r="D76" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="E76" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="72" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>163</v>
       </c>
@@ -2582,8 +2654,11 @@
       <c r="D77" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E77" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>165</v>
       </c>
@@ -2595,6 +2670,9 @@
       </c>
       <c r="D78" s="2" t="s">
         <v>77</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates to mapping table, added practitionerRole profile, updated examples, etc.
</commit_message>
<xml_diff>
--- a/mapping/Mappings.xlsx
+++ b/mapping/Mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62771155-8ECC-4F13-B75C-68F0D5EFFA8E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E35DE7-F1B6-4A00-841C-9D090940296B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" activeTab="1" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
   </bookViews>
   <sheets>
     <sheet name="RR" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="363">
   <si>
     <t>Date and time of eICR Receipt</t>
   </si>
@@ -535,9 +535,6 @@
     <t>Reportability Response Coded Information Organizer/Relevant Reportable Condition Observation/Reportability Information Organizer/Rules Authoring Agency/participantRole/playingEntity/name</t>
   </si>
   <si>
-    <t>FHIR</t>
-  </si>
-  <si>
     <t>Reportability Response/effectiveTime</t>
   </si>
   <si>
@@ -892,15 +889,6 @@
     <t>3284-264</t>
   </si>
   <si>
-    <t>us-core-patient.extension:us-core-ethnicity</t>
-  </si>
-  <si>
-    <t>us-core-patient.extension:us-core-race</t>
-  </si>
-  <si>
-    <t>us-core-patient.extension:us-core-birthsex</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
@@ -910,130 +898,229 @@
     <t>Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Working on this </t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation(PlanDefinition).contentReference: rr-plandefinition.extension-rr-determination-of-reportability-reason</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.contentReference:rr-plandefinition.extension-rr-determination-of-reportability-rule</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.contentReference: rr-plandefinition.extension-rr-determination-of-reportability</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceEICRInformation.contentReference.identifier</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).context: eicr-encounter.id</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceEICRInformation.extension-rr-eicr-processing-status</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-location-relevance</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).action.documentation.extension-rr-external-resource-priority</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).action.documentation.url</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).action.documentation.display</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).action.documentation.extension-rr-external-resource-type</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).goal.address.coding.display</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).goal.address.coding.code</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).topic.display</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceReportabilityResponseSummary.contentString</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).identifier</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).timingDuration</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).subject.us-core-patient (Patient).gender</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).subject.us-core-patient (Patient).birthdate</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).subject.us-core-patient (Patient).us-core-ethnicity</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).subject.us-core-patient (Patient).us-core-race</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).subject.us-core-patient (Patient).identifier</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).subject.us-core-patient (Patient).name</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).subject.us-core-patient (Patient).communication.language</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload: sliceEICRInformation.extension-rr-manually-initiated-eicr</t>
-  </si>
-  <si>
     <t>Clinical Document/record target/patientRole/patient/guardian/guardianPerson/name</t>
   </si>
   <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-responsible-agency.rr-responsible-agency (US Core Organization).telecom</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-responsible-agency.rr-responsible-agency (US Core Organization).address</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-routing-entity.rr-routing-entity (US Core Organization).address</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-responsible-agency.rr-responsible-agency (US Core Organization).text</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-responsible-agency.rr-responsible-agency (US Core Organization).identifier</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-responsible-agency.rr-responsible-agency (US Core Organization).name</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-routing-entity.rr-routing-entity (US Core Organization).text</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-routing-entity.rr-routing-entity (US Core Organization).identifier</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-routing-entity.rr-routing-entity (US Core Organization).name</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-routing-entity.rr-routing-entity (US Core Organization).telecom</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-rules-authoring-agency.rr-rules-authoring-agency (US Core Organization).address</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-rules-authoring-agency.rr-rules-authoring-agency (US Core Organization).telecom</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-rules-authoring-agency.rr-rules-authoring-agency (US Core Organization).text</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-rules-authoring-agency.rr-rules-authoring-agency (US Core Organization).identifier</t>
-  </si>
-  <si>
-    <t>rr-communication (Communication).payload:sliceRelevantReportableConditionInformation.rr-plandefinition (PlanDefinition).jurisdiction.extension-rr-rules-authoring-agency.rr-rules-authoring-agency (US Core Organization).name</t>
+    <t>Communication[rr-communication]</t>
+  </si>
+  <si>
+    <t>payload: sliceEICRInformation.contentReference.identifier</t>
+  </si>
+  <si>
+    <t>extension-rr-determination-of-reportability-reason</t>
+  </si>
+  <si>
+    <t>PlanDefinition[rr-plandefinition]</t>
+  </si>
+  <si>
+    <t>extension-rr-determination-of-reportability-rule</t>
+  </si>
+  <si>
+    <t>extension-rr-determination-of-reportability</t>
+  </si>
+  <si>
+    <t>context:eicr-encounter.identifier</t>
+  </si>
+  <si>
+    <t>Observation[eicr-processing-status]</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Observation[eicr-processing-status-reason]</t>
+  </si>
+  <si>
+    <t>FHIR Resource</t>
+  </si>
+  <si>
+    <t>valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>extension.valueAttachment</t>
+  </si>
+  <si>
+    <t>extension.valueString, extension.valueMarkdown</t>
+  </si>
+  <si>
+    <t>action.documentation.extension-rr-external-resource-type</t>
+  </si>
+  <si>
+    <t>action.documentation.extension-rr-external-resource-priority</t>
+  </si>
+  <si>
+    <t>action.documentation.url</t>
+  </si>
+  <si>
+    <t>action.documentation.display</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>jurisdiction.extension-rr-location-relevance</t>
+  </si>
+  <si>
+    <t>payload: sliceEICRInformation.extension-rr-manually-initiated-eicr</t>
+  </si>
+  <si>
+    <t>component[code="RRVS33"].valueString</t>
+  </si>
+  <si>
+    <t>component[code="RRVS32"].valueCode</t>
+  </si>
+  <si>
+    <t>component[code="RRVS31"].valueCode</t>
+  </si>
+  <si>
+    <t>Patient[us-core-patient]</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>birthdate</t>
+  </si>
+  <si>
+    <t>us-core-ethnicity</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>communication.language</t>
+  </si>
+  <si>
+    <t>us-core-race</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>telecom[system="phone"]</t>
+  </si>
+  <si>
+    <t>telecom[system="email"]</t>
+  </si>
+  <si>
+    <t>telecom[system="fax']</t>
+  </si>
+  <si>
+    <t>goal.address.coding.display</t>
+  </si>
+  <si>
+    <t>goal.address.coding.code</t>
+  </si>
+  <si>
+    <t>topic.display</t>
+  </si>
+  <si>
+    <t>payload: sliceReportabilityResponseSummary.contentString</t>
+  </si>
+  <si>
+    <t>timingDuration</t>
+  </si>
+  <si>
+    <t>Organization[rr-responsible-agency]</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Organization[rr-routing-entity]</t>
+  </si>
+  <si>
+    <t>Organization[rr-rules-authoring-agency]</t>
+  </si>
+  <si>
+    <t>Communication[rr-communication].payload</t>
+  </si>
+  <si>
+    <t>PlanDefinition[rr-plandefinition].extension</t>
+  </si>
+  <si>
+    <t>Observation[eicr-processing-status].related</t>
+  </si>
+  <si>
+    <t>Communication[rr-communication].subject</t>
+  </si>
+  <si>
+    <t>FHIR Contained by</t>
+  </si>
+  <si>
+    <t>PlanDefinition[rr-plandefinition].jurisdiction</t>
+  </si>
+  <si>
+    <t>PlanDefinition[rr-plandefinition].publisher</t>
+  </si>
+  <si>
+    <t>FHIR Element Path</t>
+  </si>
+  <si>
+    <t>Communication[rr-communication].recipient</t>
+  </si>
+  <si>
+    <t>Practitioner[us-core-practitioner]</t>
+  </si>
+  <si>
+    <t>Encounter[eicr-encounter].location</t>
+  </si>
+  <si>
+    <t>Location[eicr-location]</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>telecom[system="fax"]</t>
+  </si>
+  <si>
+    <t>contact.telecom[system="email"]</t>
+  </si>
+  <si>
+    <t>contact.name</t>
+  </si>
+  <si>
+    <t>contact.telecom[system="phone"]</t>
+  </si>
+  <si>
+    <t>PractitionerRole.organization</t>
+  </si>
+  <si>
+    <t>Organization[eicr-organization]</t>
+  </si>
+  <si>
+    <t>Composition[eicr-composition]</t>
+  </si>
+  <si>
+    <t>Composition[eicr-composition].subject</t>
+  </si>
+  <si>
+    <t>us-core-birthsex</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Encounter[eicr-encounter].participant[type="ATND"].PractitionerRole[ecr-practitionerrole].practitioner</t>
+  </si>
+  <si>
+    <t>Encounter[eicr-encounter].participant[type="ATND"].PractitionerRole[ecr-practitionerrole].location</t>
+  </si>
+  <si>
+    <t>Location(eicr-location)</t>
+  </si>
+  <si>
+    <t>Composition[eicr-composition].section</t>
+  </si>
+  <si>
+    <t>Observation[eicr-occupationhistory]</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1090,6 +1177,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1103,7 +1196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1111,7 +1204,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1128,6 +1220,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1442,47 +1555,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2E64F1-05B1-4B7F-9A17-F737E551CA1E}">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B73" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C77" sqref="C77"/>
+      <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="77.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.140625" style="3"/>
-    <col min="4" max="4" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="21" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="77.140625" style="3"/>
+    <col min="1" max="1" width="36.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.140625" style="4"/>
+    <col min="4" max="4" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="77.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1495,8 +1620,10 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1509,11 +1636,18 @@
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+      <c r="E3" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1526,11 +1660,18 @@
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+      <c r="E4" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1543,11 +1684,18 @@
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="E5" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1560,11 +1708,18 @@
       <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1577,11 +1732,14 @@
       <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1594,11 +1752,14 @@
       <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1611,14 +1772,19 @@
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E9" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1631,14 +1797,19 @@
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E10" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1651,14 +1822,19 @@
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E11" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -1671,14 +1847,19 @@
       <c r="D12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E12" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>35</v>
       </c>
@@ -1691,14 +1872,19 @@
       <c r="D13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E13" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
@@ -1711,14 +1897,19 @@
       <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="E14" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -1731,11 +1922,18 @@
       <c r="D15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+      <c r="E15" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1748,11 +1946,18 @@
       <c r="D16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="E16" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
@@ -1765,11 +1970,18 @@
       <c r="D17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="E17" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -1782,11 +1994,18 @@
       <c r="D18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="E18" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
@@ -1799,8 +2018,17 @@
       <c r="D19" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -1813,8 +2041,17 @@
       <c r="D20" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="E20" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -1827,8 +2064,17 @@
       <c r="D21" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="E21" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
@@ -1841,8 +2087,17 @@
       <c r="D22" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="E22" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>60</v>
       </c>
@@ -1855,8 +2110,17 @@
       <c r="D23" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -1869,8 +2133,17 @@
       <c r="D24" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>64</v>
       </c>
@@ -1883,8 +2156,11 @@
       <c r="D25" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>66</v>
       </c>
@@ -1897,8 +2173,17 @@
       <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="E26" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>68</v>
       </c>
@@ -1911,11 +2196,18 @@
       <c r="D27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+      <c r="E27" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>70</v>
       </c>
@@ -1928,11 +2220,18 @@
       <c r="D28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>72</v>
       </c>
@@ -1945,8 +2244,17 @@
       <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -1959,8 +2267,17 @@
       <c r="D30" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>76</v>
       </c>
@@ -1968,13 +2285,22 @@
         <v>22</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>318</v>
+        <v>288</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>78</v>
       </c>
@@ -1987,8 +2313,17 @@
       <c r="D32" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="E32" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>80</v>
       </c>
@@ -2001,11 +2336,18 @@
       <c r="D33" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="E33" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>82</v>
       </c>
@@ -2018,11 +2360,18 @@
       <c r="D34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>84</v>
       </c>
@@ -2035,8 +2384,17 @@
       <c r="D35" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="E35" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>86</v>
       </c>
@@ -2049,11 +2407,18 @@
       <c r="D36" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="E36" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>88</v>
       </c>
@@ -2066,11 +2431,18 @@
       <c r="D37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F37" s="12" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="G37" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>90</v>
       </c>
@@ -2083,11 +2455,18 @@
       <c r="D38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>92</v>
       </c>
@@ -2100,8 +2479,17 @@
       <c r="D39" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="E39" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>94</v>
       </c>
@@ -2114,11 +2502,18 @@
       <c r="D40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="E40" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>96</v>
       </c>
@@ -2131,11 +2526,18 @@
       <c r="D41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>98</v>
       </c>
@@ -2148,162 +2550,251 @@
       <c r="D42" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+      <c r="E42" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
+      <c r="E43" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D44" s="9"/>
-    </row>
-    <row r="45" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+      <c r="D44" s="8"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="14"/>
+    </row>
+    <row r="45" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
+      <c r="E45" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="G45" s="14" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
       <c r="C46" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D46" s="9"/>
-    </row>
-    <row r="47" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="D46" s="8"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="14"/>
+    </row>
+    <row r="47" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
+      <c r="E47" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="G47" s="17" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D48" s="9"/>
-    </row>
-    <row r="49" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="D48" s="8"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="17"/>
+    </row>
+    <row r="49" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D49" s="9" t="s">
+      <c r="D49" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
+      <c r="E49" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="9"/>
-    </row>
-    <row r="51" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="D50" s="8"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+    </row>
+    <row r="51" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A51" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
-      <c r="B52" s="9"/>
+      <c r="E51" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
       <c r="C52" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="9"/>
-    </row>
-    <row r="53" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+      <c r="D52" s="8"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+    </row>
+    <row r="53" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D53" s="9" t="s">
+      <c r="D53" s="8" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
+      <c r="E53" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
       <c r="C54" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D54" s="9"/>
-    </row>
-    <row r="55" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+      <c r="D54" s="8"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+    </row>
+    <row r="55" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D55" s="9" t="s">
+      <c r="D55" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
+      <c r="E55" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
       <c r="C56" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D56" s="9"/>
-    </row>
-    <row r="57" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+      <c r="D56" s="8"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>121</v>
       </c>
@@ -2314,11 +2805,18 @@
         <v>122</v>
       </c>
       <c r="D57" s="2"/>
-      <c r="E57" s="4" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+      <c r="E57" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>123</v>
       </c>
@@ -2331,11 +2829,18 @@
       <c r="D58" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="4" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E58" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>125</v>
       </c>
@@ -2348,11 +2853,14 @@
       <c r="D59" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F59" s="4" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="16"/>
+      <c r="I59" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>127</v>
       </c>
@@ -2365,11 +2873,18 @@
       <c r="D60" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E60" s="4" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="E60" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="H60" s="3"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>130</v>
       </c>
@@ -2382,11 +2897,18 @@
       <c r="D61" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E61" s="4" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E61" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="H61" s="3"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>132</v>
       </c>
@@ -2399,11 +2921,18 @@
       <c r="D62" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E62" s="4" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="E62" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="H62" s="3"/>
+    </row>
+    <row r="63" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>134</v>
       </c>
@@ -2416,11 +2945,18 @@
       <c r="D63" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E63" s="4" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="E63" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="H63" s="3"/>
+    </row>
+    <row r="64" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>137</v>
       </c>
@@ -2433,11 +2969,18 @@
       <c r="D64" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E64" s="4" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="E64" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="H64" s="3"/>
+    </row>
+    <row r="65" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>139</v>
       </c>
@@ -2450,11 +2993,18 @@
       <c r="D65" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E65" s="4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="E65" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="H65" s="3"/>
+    </row>
+    <row r="66" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>141</v>
       </c>
@@ -2467,11 +3017,18 @@
       <c r="D66" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E66" s="4" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="E66" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="H66" s="3"/>
+    </row>
+    <row r="67" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>143</v>
       </c>
@@ -2484,11 +3041,18 @@
       <c r="D67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E67" s="4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="E67" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="H67" s="3"/>
+    </row>
+    <row r="68" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>145</v>
       </c>
@@ -2501,11 +3065,18 @@
       <c r="D68" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E68" s="4" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="E68" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="H68" s="3"/>
+    </row>
+    <row r="69" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>147</v>
       </c>
@@ -2518,11 +3089,18 @@
       <c r="D69" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E69" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="G69" s="11" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="H69" s="3"/>
+    </row>
+    <row r="70" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>149</v>
       </c>
@@ -2535,11 +3113,18 @@
       <c r="D70" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E70" s="4" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="E70" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>151</v>
       </c>
@@ -2552,11 +3137,18 @@
       <c r="D71" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E71" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="E71" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>153</v>
       </c>
@@ -2569,11 +3161,18 @@
       <c r="D72" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E72" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="E72" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>155</v>
       </c>
@@ -2586,11 +3185,18 @@
       <c r="D73" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E73" s="4" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="E73" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>157</v>
       </c>
@@ -2603,11 +3209,18 @@
       <c r="D74" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E74" s="4" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="E74" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="H74" s="3"/>
+    </row>
+    <row r="75" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>159</v>
       </c>
@@ -2620,11 +3233,18 @@
       <c r="D75" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E75" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="E75" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="H75" s="3"/>
+    </row>
+    <row r="76" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>161</v>
       </c>
@@ -2637,11 +3257,18 @@
       <c r="D76" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E76" s="4" t="s">
+      <c r="E76" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="G76" s="11" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="H76" s="3"/>
+    </row>
+    <row r="77" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>163</v>
       </c>
@@ -2654,11 +3281,18 @@
       <c r="D77" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E77" s="4" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="E77" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="G77" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="H77" s="3"/>
+    </row>
+    <row r="78" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>165</v>
       </c>
@@ -2671,31 +3305,54 @@
       <c r="D78" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E78" s="4" t="s">
+      <c r="E78" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="F78" s="10" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C79" s="4" t="s">
+      <c r="G78" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="H78" s="3"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C79" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G79" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="E79" s="3" t="s">
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C80" s="3" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C80" s="4" t="s">
+      <c r="G80" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="I80" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E80" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>171</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="37">
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="D43:D44"/>
@@ -2725,858 +3382,1105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1E071C-8572-48FD-94ED-9BC2BF0CD944}">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.42578125" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="23.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="44" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>179</v>
-      </c>
       <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="E3" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="E4" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="E5" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="E6" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="36" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="E8" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="E9" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="E10" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="E11" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="E12" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="B14" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B16" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
+      <c r="B24" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="D24" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="2" t="s">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2"/>
+      <c r="E26" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
+      <c r="B28" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D29" s="9"/>
-    </row>
-    <row r="30" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="D32" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>221</v>
+      <c r="E32" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
       <c r="D33" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D35" s="6"/>
+        <v>190</v>
+      </c>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>233</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="D40" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>242</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="8"/>
+      <c r="B54" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="9"/>
-      <c r="B54" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="D54" s="9"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="9" t="s">
+      <c r="D55" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B55" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>264</v>
-      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
       <c r="D56" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+      <c r="B58" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="36" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>272</v>
-      </c>
       <c r="D59" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="1:4" ht="36" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
+      <c r="B63" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>281</v>
       </c>
       <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="1:4" ht="36" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
+      <c r="B65" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="D65" s="2"/>
     </row>

</xml_diff>

<commit_message>
Changes to mapping table and eicr-location
</commit_message>
<xml_diff>
--- a/mapping/Mappings.xlsx
+++ b/mapping/Mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E35DE7-F1B6-4A00-841C-9D090940296B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DA76C2-E6CD-407A-885A-77803B388716}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" activeTab="1" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
   </bookViews>
   <sheets>
     <sheet name="RR" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="364">
   <si>
     <t>Date and time of eICR Receipt</t>
   </si>
@@ -1121,6 +1121,9 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>TODO</t>
   </si>
 </sst>
 </file>
@@ -1217,9 +1220,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1230,17 +1230,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1557,11 +1560,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2E64F1-05B1-4B7F-9A17-F737E551CA1E}">
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="77.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1570,9 +1573,9 @@
     <col min="2" max="2" width="33.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="77.140625" style="4"/>
     <col min="4" max="4" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="48.5703125" style="4" customWidth="1"/>
     <col min="9" max="9" width="21" style="4" customWidth="1"/>
     <col min="10" max="16384" width="77.140625" style="4"/>
@@ -1591,13 +1594,13 @@
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>341</v>
       </c>
       <c r="H1" s="7" t="s">
@@ -1620,8 +1623,8 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1636,13 +1639,13 @@
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>291</v>
       </c>
       <c r="H3" s="3"/>
@@ -1660,13 +1663,13 @@
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>293</v>
       </c>
       <c r="H4" s="3"/>
@@ -1684,13 +1687,13 @@
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>294</v>
       </c>
       <c r="H5" s="3"/>
@@ -1708,13 +1711,13 @@
       <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
         <v>290</v>
       </c>
       <c r="H6" s="3"/>
@@ -1732,9 +1735,9 @@
       <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="11" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="10" t="s">
         <v>285</v>
       </c>
       <c r="H7" s="3"/>
@@ -1752,9 +1755,9 @@
       <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="11" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="10" t="s">
         <v>285</v>
       </c>
       <c r="H8" s="3"/>
@@ -1772,13 +1775,13 @@
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="10" t="s">
         <v>295</v>
       </c>
       <c r="H9" s="3"/>
@@ -1797,13 +1800,13 @@
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="10" t="s">
         <v>297</v>
       </c>
       <c r="H10" s="3"/>
@@ -1822,13 +1825,13 @@
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="10" t="s">
         <v>301</v>
       </c>
       <c r="H11" s="3"/>
@@ -1847,13 +1850,13 @@
       <c r="D12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="10" t="s">
         <v>303</v>
       </c>
       <c r="H12" s="3"/>
@@ -1872,13 +1875,13 @@
       <c r="D13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="10" t="s">
         <v>302</v>
       </c>
       <c r="H13" s="3"/>
@@ -1897,13 +1900,13 @@
       <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="10" t="s">
         <v>311</v>
       </c>
       <c r="H14" s="3"/>
@@ -1922,13 +1925,13 @@
       <c r="D15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="10" t="s">
         <v>304</v>
       </c>
       <c r="H15" s="3"/>
@@ -1946,13 +1949,13 @@
       <c r="D16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>307</v>
       </c>
       <c r="H16" s="3"/>
@@ -1970,13 +1973,13 @@
       <c r="D17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>306</v>
       </c>
       <c r="H17" s="3"/>
@@ -1994,13 +1997,13 @@
       <c r="D18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="10" t="s">
         <v>305</v>
       </c>
       <c r="H18" s="3"/>
@@ -2018,13 +2021,13 @@
       <c r="D19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="9" t="s">
         <v>321</v>
       </c>
     </row>
@@ -2041,13 +2044,13 @@
       <c r="D20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="9" t="s">
         <v>318</v>
       </c>
     </row>
@@ -2064,13 +2067,13 @@
       <c r="D21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>298</v>
       </c>
     </row>
@@ -2087,13 +2090,13 @@
       <c r="D22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="9" t="s">
         <v>347</v>
       </c>
     </row>
@@ -2110,13 +2113,13 @@
       <c r="D23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="9" t="s">
         <v>322</v>
       </c>
     </row>
@@ -2133,13 +2136,13 @@
       <c r="D24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="9" t="s">
         <v>346</v>
       </c>
     </row>
@@ -2156,9 +2159,11 @@
       <c r="D25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="13" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
@@ -2173,13 +2178,13 @@
       <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="10" t="s">
         <v>312</v>
       </c>
     </row>
@@ -2196,13 +2201,13 @@
       <c r="D27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="10" t="s">
         <v>309</v>
       </c>
       <c r="H27" s="3"/>
@@ -2220,13 +2225,13 @@
       <c r="D28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="10" t="s">
         <v>310</v>
       </c>
       <c r="H28" s="3"/>
@@ -2244,13 +2249,13 @@
       <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="10" t="s">
         <v>313</v>
       </c>
     </row>
@@ -2267,13 +2272,13 @@
       <c r="D30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="G30" s="9" t="s">
         <v>348</v>
       </c>
     </row>
@@ -2290,13 +2295,13 @@
       <c r="D31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="9" t="s">
         <v>349</v>
       </c>
     </row>
@@ -2313,13 +2318,13 @@
       <c r="D32" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="9" t="s">
         <v>350</v>
       </c>
     </row>
@@ -2336,13 +2341,13 @@
       <c r="D33" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" s="10" t="s">
         <v>315</v>
       </c>
       <c r="H33" s="3"/>
@@ -2360,13 +2365,13 @@
       <c r="D34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="10" t="s">
         <v>316</v>
       </c>
       <c r="H34" s="3"/>
@@ -2384,13 +2389,13 @@
       <c r="D35" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F35" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="10" t="s">
         <v>323</v>
       </c>
     </row>
@@ -2407,13 +2412,13 @@
       <c r="D36" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G36" s="10" t="s">
         <v>317</v>
       </c>
       <c r="H36" s="3"/>
@@ -2431,13 +2436,13 @@
       <c r="D37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G37" s="10" t="s">
         <v>318</v>
       </c>
       <c r="H37" s="3"/>
@@ -2455,13 +2460,13 @@
       <c r="D38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F38" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G38" s="10" t="s">
         <v>298</v>
       </c>
       <c r="H38" s="3"/>
@@ -2479,13 +2484,13 @@
       <c r="D39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="F39" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="G39" s="10" t="s">
         <v>322</v>
       </c>
     </row>
@@ -2502,13 +2507,13 @@
       <c r="D40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="G40" s="10" t="s">
         <v>319</v>
       </c>
       <c r="H40" s="3"/>
@@ -2526,13 +2531,13 @@
       <c r="D41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="G41" s="10" t="s">
         <v>320</v>
       </c>
       <c r="H41" s="3"/>
@@ -2550,249 +2555,249 @@
       <c r="D42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G42" s="11" t="s">
+      <c r="G42" s="10" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E43" s="13" t="s">
+      <c r="E43" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="F43" s="13" t="s">
+      <c r="F43" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="G43" s="14" t="s">
+      <c r="G43" s="16" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
       <c r="C44" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="14"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="16"/>
     </row>
     <row r="45" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E45" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="F45" s="13" t="s">
+      <c r="F45" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="G45" s="16" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
       <c r="C46" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="14"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="16"/>
     </row>
     <row r="47" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="E47" s="16" t="s">
         <v>351</v>
       </c>
-      <c r="F47" s="14" t="s">
+      <c r="F47" s="16" t="s">
         <v>352</v>
       </c>
-      <c r="G47" s="17" t="s">
+      <c r="G47" s="14" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="14"/>
     </row>
     <row r="49" spans="1:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="E49" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="F49" s="13" t="s">
+      <c r="F49" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="G49" s="10" t="s">
+      <c r="G49" s="9" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
       <c r="C50" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
     </row>
     <row r="51" spans="1:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E51" s="13" t="s">
+      <c r="E51" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="F51" s="13" t="s">
+      <c r="F51" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="G51" s="10" t="s">
+      <c r="G51" s="9" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
       <c r="C52" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
     </row>
     <row r="53" spans="1:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E53" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="F53" s="13" t="s">
+      <c r="F53" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="G53" s="10" t="s">
+      <c r="G53" s="9" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
+      <c r="A54" s="17"/>
+      <c r="B54" s="17"/>
       <c r="C54" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D54" s="8"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
     </row>
     <row r="55" spans="1:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E55" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="F55" s="13" t="s">
+      <c r="F55" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="G55" s="10" t="s">
+      <c r="G55" s="9" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
       <c r="C56" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
@@ -2805,13 +2810,13 @@
         <v>122</v>
       </c>
       <c r="D57" s="2"/>
-      <c r="E57" s="12" t="s">
+      <c r="E57" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="F57" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="G57" s="11" t="s">
+      <c r="G57" s="10" t="s">
         <v>325</v>
       </c>
       <c r="H57" s="3"/>
@@ -2829,13 +2834,13 @@
       <c r="D58" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E58" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="G58" s="11" t="s">
+      <c r="G58" s="10" t="s">
         <v>326</v>
       </c>
       <c r="H58" s="3"/>
@@ -2853,9 +2858,11 @@
       <c r="D59" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="16"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="13" t="s">
+        <v>363</v>
+      </c>
       <c r="I59" s="3" t="s">
         <v>286</v>
       </c>
@@ -2873,13 +2880,13 @@
       <c r="D60" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E60" s="12" t="s">
+      <c r="E60" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F60" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="G60" s="11" t="s">
+      <c r="G60" s="10" t="s">
         <v>327</v>
       </c>
       <c r="H60" s="3"/>
@@ -2897,13 +2904,13 @@
       <c r="D61" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E61" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F61" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="G61" s="11" t="s">
+      <c r="G61" s="10" t="s">
         <v>328</v>
       </c>
       <c r="H61" s="3"/>
@@ -2921,13 +2928,13 @@
       <c r="D62" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E62" s="12" t="s">
+      <c r="E62" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="F62" s="12" t="s">
+      <c r="F62" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="G62" s="11" t="s">
+      <c r="G62" s="10" t="s">
         <v>318</v>
       </c>
       <c r="H62" s="3"/>
@@ -2945,13 +2952,13 @@
       <c r="D63" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E63" s="12" t="s">
+      <c r="E63" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="F63" s="12" t="s">
+      <c r="F63" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="G63" s="11" t="s">
+      <c r="G63" s="10" t="s">
         <v>329</v>
       </c>
       <c r="H63" s="3"/>
@@ -2969,13 +2976,13 @@
       <c r="D64" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="F64" s="10" t="s">
+      <c r="F64" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="G64" s="11" t="s">
+      <c r="G64" s="10" t="s">
         <v>321</v>
       </c>
       <c r="H64" s="3"/>
@@ -2993,13 +3000,13 @@
       <c r="D65" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E65" s="12" t="s">
+      <c r="E65" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="F65" s="10" t="s">
+      <c r="F65" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="G65" s="11" t="s">
+      <c r="G65" s="10" t="s">
         <v>322</v>
       </c>
       <c r="H65" s="3"/>
@@ -3017,13 +3024,13 @@
       <c r="D66" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="F66" s="10" t="s">
+      <c r="F66" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="G66" s="11" t="s">
+      <c r="G66" s="10" t="s">
         <v>331</v>
       </c>
       <c r="H66" s="3"/>
@@ -3041,13 +3048,13 @@
       <c r="D67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E67" s="12" t="s">
+      <c r="E67" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="F67" s="10" t="s">
+      <c r="F67" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="G67" s="11" t="s">
+      <c r="G67" s="10" t="s">
         <v>318</v>
       </c>
       <c r="H67" s="3"/>
@@ -3065,13 +3072,13 @@
       <c r="D68" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E68" s="12" t="s">
+      <c r="E68" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="F68" s="10" t="s">
+      <c r="F68" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="G68" s="11" t="s">
+      <c r="G68" s="10" t="s">
         <v>298</v>
       </c>
       <c r="H68" s="3"/>
@@ -3089,13 +3096,13 @@
       <c r="D69" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E69" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="F69" s="10" t="s">
+      <c r="F69" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="G69" s="11" t="s">
+      <c r="G69" s="10" t="s">
         <v>321</v>
       </c>
       <c r="H69" s="3"/>
@@ -3113,13 +3120,13 @@
       <c r="D70" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E70" s="12" t="s">
+      <c r="E70" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="F70" s="10" t="s">
+      <c r="F70" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="G70" s="11" t="s">
+      <c r="G70" s="10" t="s">
         <v>322</v>
       </c>
       <c r="H70" s="3"/>
@@ -3137,13 +3144,13 @@
       <c r="D71" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E71" s="12" t="s">
+      <c r="E71" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="F71" s="10" t="s">
+      <c r="F71" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="G71" s="11" t="s">
+      <c r="G71" s="10" t="s">
         <v>331</v>
       </c>
       <c r="H71" s="3"/>
@@ -3161,13 +3168,13 @@
       <c r="D72" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E72" s="12" t="s">
+      <c r="E72" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="F72" s="10" t="s">
+      <c r="F72" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="G72" s="11" t="s">
+      <c r="G72" s="10" t="s">
         <v>318</v>
       </c>
       <c r="H72" s="3"/>
@@ -3185,13 +3192,13 @@
       <c r="D73" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E73" s="12" t="s">
+      <c r="E73" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="F73" s="10" t="s">
+      <c r="F73" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="G73" s="11" t="s">
+      <c r="G73" s="10" t="s">
         <v>298</v>
       </c>
       <c r="H73" s="3"/>
@@ -3209,13 +3216,13 @@
       <c r="D74" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E74" s="12" t="s">
+      <c r="E74" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="F74" s="10" t="s">
+      <c r="F74" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="G74" s="11" t="s">
+      <c r="G74" s="10" t="s">
         <v>321</v>
       </c>
       <c r="H74" s="3"/>
@@ -3233,13 +3240,13 @@
       <c r="D75" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E75" s="12" t="s">
+      <c r="E75" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="F75" s="10" t="s">
+      <c r="F75" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="G75" s="11" t="s">
+      <c r="G75" s="10" t="s">
         <v>322</v>
       </c>
       <c r="H75" s="3"/>
@@ -3257,13 +3264,13 @@
       <c r="D76" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E76" s="12" t="s">
+      <c r="E76" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="F76" s="10" t="s">
+      <c r="F76" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="G76" s="11" t="s">
+      <c r="G76" s="10" t="s">
         <v>331</v>
       </c>
       <c r="H76" s="3"/>
@@ -3281,13 +3288,13 @@
       <c r="D77" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E77" s="12" t="s">
+      <c r="E77" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="F77" s="10" t="s">
+      <c r="F77" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="G77" s="11" t="s">
+      <c r="G77" s="10" t="s">
         <v>318</v>
       </c>
       <c r="H77" s="3"/>
@@ -3305,13 +3312,13 @@
       <c r="D78" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E78" s="12" t="s">
+      <c r="E78" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="F78" s="10" t="s">
+      <c r="F78" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="G78" s="11" t="s">
+      <c r="G78" s="10" t="s">
         <v>298</v>
       </c>
       <c r="H78" s="3"/>
@@ -3320,7 +3327,7 @@
       <c r="C79" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="G79" s="10" t="s">
+      <c r="G79" s="9" t="s">
         <v>168</v>
       </c>
     </row>
@@ -3328,7 +3335,7 @@
       <c r="C80" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="G80" s="10" t="s">
+      <c r="G80" s="9" t="s">
         <v>171</v>
       </c>
       <c r="I80" s="4" t="s">
@@ -3337,6 +3344,33 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
     <mergeCell ref="E53:E54"/>
     <mergeCell ref="F53:F54"/>
     <mergeCell ref="E55:E56"/>
@@ -3347,33 +3381,6 @@
     <mergeCell ref="F49:F50"/>
     <mergeCell ref="E51:E52"/>
     <mergeCell ref="F51:F52"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:D54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3384,11 +3391,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1E071C-8572-48FD-94ED-9BC2BF0CD944}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D52" sqref="D52"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3414,13 +3421,13 @@
       <c r="D1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>341</v>
       </c>
     </row>
@@ -3435,11 +3442,11 @@
         <v>178</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>356</v>
       </c>
     </row>
@@ -3459,10 +3466,10 @@
       <c r="E3" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3480,7 +3487,7 @@
       <c r="E4" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>343</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -3503,7 +3510,7 @@
       <c r="E5" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>343</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -3526,7 +3533,7 @@
       <c r="E6" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>343</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -3549,7 +3556,7 @@
       <c r="E7" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>343</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -3570,7 +3577,7 @@
       <c r="E8" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>345</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -3591,7 +3598,7 @@
       <c r="E9" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>343</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -3850,10 +3857,10 @@
       <c r="E21" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>349</v>
       </c>
     </row>
@@ -3873,10 +3880,10 @@
       <c r="E22" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="9" t="s">
         <v>350</v>
       </c>
     </row>
@@ -3896,21 +3903,21 @@
       <c r="E23" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="9" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="17" t="s">
         <v>202</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -3919,7 +3926,7 @@
       <c r="E24" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="11" t="s">
         <v>314</v>
       </c>
       <c r="G24" s="4" t="s">
@@ -3927,9 +3934,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="2" t="s">
         <v>203</v>
       </c>
@@ -3948,7 +3955,7 @@
       <c r="E26" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="11" t="s">
         <v>314</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -3971,7 +3978,7 @@
       <c r="E27" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>314</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -3979,22 +3986,22 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="17" t="s">
         <v>177</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="17" t="s">
         <v>181</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="11" t="s">
         <v>314</v>
       </c>
       <c r="G28" s="4" t="s">
@@ -4002,12 +4009,12 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D29" s="8"/>
+      <c r="D29" s="17"/>
     </row>
     <row r="30" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
@@ -4025,7 +4032,7 @@
       <c r="E30" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="11" t="s">
         <v>314</v>
       </c>
       <c r="G30" s="4" t="s">
@@ -4048,21 +4055,21 @@
       <c r="E31" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="10" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="17" t="s">
         <v>219</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -4079,9 +4086,9 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="2" t="s">
         <v>181</v>
       </c>
@@ -4211,13 +4218,13 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="17" t="s">
         <v>245</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -4225,21 +4232,21 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
       <c r="D44" s="2" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="17" t="s">
         <v>248</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -4247,41 +4254,41 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
       <c r="D46" s="2" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="C47" s="8"/>
+      <c r="C47" s="17"/>
       <c r="D47" s="2" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
       <c r="D48" s="2" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="17" t="s">
         <v>253</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -4289,9 +4296,9 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
       <c r="D50" s="2" t="s">
         <v>181</v>
       </c>
@@ -4325,7 +4332,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="17" t="s">
         <v>258</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -4334,28 +4341,28 @@
       <c r="C53" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="17" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="8"/>
+      <c r="A54" s="17"/>
       <c r="B54" s="2" t="s">
         <v>247</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D54" s="8"/>
+      <c r="D54" s="17"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="17" t="s">
         <v>223</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -4363,9 +4370,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
       <c r="D56" s="2" t="s">
         <v>181</v>
       </c>
@@ -4486,18 +4493,7 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D53:D54"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="C55:C56"/>
@@ -4511,7 +4507,18 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="A53:A54"/>
-    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4519,15 +4526,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E2A70C0F482D004F81B909595C75DFA6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e14e4ad0a6f5f1a0ddcbf041a2a4a832">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="9ed5a28f-e285-4793-933e-f86572ea3e88" xmlns:ns3="6FDAA894-E433-443A-929C-6668B5175CA9" xmlns:ns4="a130c0bc-081d-4a7d-8c4b-0d956631a56e" xmlns:ns5="6fdaa894-e433-443a-929c-6668b5175ca9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f3fa50635c17e9cfabaeee8fe605afa8" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4732,6 +4730,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4746,14 +4753,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{211F509A-75D2-471F-BE44-DEEBD2FE04CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28D2A50F-394A-4741-95EF-7EE6194A4F57}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4775,20 +4774,28 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{211F509A-75D2-471F-BE44-DEEBD2FE04CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B0C849C-1E0C-4B3D-9203-5FFDB8062BA1}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="6fdaa894-e433-443a-929c-6668b5175ca9"/>
+    <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6FDAA894-E433-443A-929C-6668B5175CA9"/>
+    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6FDAA894-E433-443A-929C-6668B5175CA9"/>
-    <ds:schemaRef ds:uri="6fdaa894-e433-443a-929c-6668b5175ca9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>

</xml_diff>

<commit_message>
Rename priority value set, add communication level priority extension, update examples
</commit_message>
<xml_diff>
--- a/mapping/Mappings.xlsx
+++ b/mapping/Mappings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\Mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DA76C2-E6CD-407A-885A-77803B388716}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EC77D7-171C-45D8-AA66-53B482D210A6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="365">
   <si>
     <t>Date and time of eICR Receipt</t>
   </si>
@@ -73,24 +73,15 @@
     <t>CD</t>
   </si>
   <si>
-    <t>eICR CDA Document ID</t>
-  </si>
-  <si>
     <t>Received eICR Information/eICR External Document Reference/id</t>
   </si>
   <si>
     <t>II</t>
   </si>
   <si>
-    <t>eICR CDA Document Set ID</t>
-  </si>
-  <si>
     <t>Received eICR Information/eICR External Document Reference/setId</t>
   </si>
   <si>
-    <t>eICR CDA Document Version Number</t>
-  </si>
-  <si>
     <t>Received eICR Information/eICR External Document Reference/versionNumber</t>
   </si>
   <si>
@@ -892,9 +883,6 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>todo</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -949,9 +937,6 @@
     <t>action.documentation.extension-rr-external-resource-type</t>
   </si>
   <si>
-    <t>action.documentation.extension-rr-external-resource-priority</t>
-  </si>
-  <si>
     <t>action.documentation.url</t>
   </si>
   <si>
@@ -1123,7 +1108,25 @@
     <t>value</t>
   </si>
   <si>
-    <t>TODO</t>
+    <t>eICR Document ID</t>
+  </si>
+  <si>
+    <t>eICR Document Set ID</t>
+  </si>
+  <si>
+    <t>eICR Document Version Number</t>
+  </si>
+  <si>
+    <t>payload: sliceEICRInformation.contentReference.display</t>
+  </si>
+  <si>
+    <t>extension-rr-priority-reason</t>
+  </si>
+  <si>
+    <t>Communication[rr-communication].extension</t>
+  </si>
+  <si>
+    <t>action.documentation.extension-rr-priority</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1177,12 +1180,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1230,10 +1227,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1243,6 +1236,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1561,10 +1560,10 @@
   <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="77.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1583,31 +1582,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1640,13 +1639,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="H3" s="3"/>
     </row>
@@ -1664,13 +1663,13 @@
         <v>7</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="H4" s="3"/>
     </row>
@@ -1688,1689 +1687,1668 @@
         <v>12</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>358</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>289</v>
-      </c>
       <c r="G6" s="10" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>359</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>360</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>289</v>
-      </c>
       <c r="G9" s="10" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>305</v>
+        <v>364</v>
       </c>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13" t="s">
-        <v>363</v>
+        <v>31</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="F28" s="10" t="s">
-        <v>289</v>
-      </c>
       <c r="G28" s="10" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F40" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="G40" s="10" t="s">
         <v>314</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>319</v>
       </c>
       <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="D43" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E42" s="11" t="s">
+      <c r="D44" s="15"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="17"/>
+    </row>
+    <row r="45" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A45" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="F42" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="2" t="s">
+      <c r="F45" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="16"/>
-    </row>
-    <row r="45" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
+      <c r="D46" s="15"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="17"/>
+    </row>
+    <row r="47" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A47" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="B47" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D45" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="F45" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="2" t="s">
+      <c r="D47" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="16"/>
-    </row>
-    <row r="47" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
+      <c r="D48" s="15"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A49" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="B47" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="B49" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>351</v>
-      </c>
-      <c r="F47" s="16" t="s">
-        <v>352</v>
-      </c>
-      <c r="G47" s="14" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="2" t="s">
+      <c r="D49" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="14"/>
-    </row>
-    <row r="49" spans="1:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
+      <c r="D50" s="15"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+    </row>
+    <row r="51" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A51" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B49" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="B51" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D49" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="2" t="s">
+      <c r="D51" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="17"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-    </row>
-    <row r="51" spans="1:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="A51" s="17" t="s">
+      <c r="D52" s="15"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+    </row>
+    <row r="53" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A53" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B51" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="B53" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D51" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="2" t="s">
+      <c r="D53" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="F53" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="17"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-    </row>
-    <row r="53" spans="1:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="A53" s="17" t="s">
+      <c r="D54" s="15"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+    </row>
+    <row r="55" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A55" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="B53" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" s="2" t="s">
+      <c r="B55" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D53" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="2" t="s">
+      <c r="D55" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="F55" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D54" s="17"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-    </row>
-    <row r="55" spans="1:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D56" s="17"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="11" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="H57" s="3"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="H58" s="3"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="13" t="s">
+      <c r="E59" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="F59" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="I59" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="G59" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="I59" s="3"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E60" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="F60" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="F60" s="11" t="s">
-        <v>289</v>
-      </c>
       <c r="G60" s="10" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E61" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="F61" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="F61" s="11" t="s">
-        <v>289</v>
-      </c>
       <c r="G61" s="10" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E62" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="F62" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="F62" s="11" t="s">
-        <v>289</v>
-      </c>
       <c r="G62" s="10" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="H63" s="3"/>
     </row>
     <row r="64" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="H64" s="3"/>
     </row>
     <row r="65" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="H65" s="3"/>
     </row>
     <row r="66" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="H66" s="3"/>
     </row>
     <row r="67" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="H67" s="3"/>
     </row>
     <row r="68" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="H68" s="3"/>
     </row>
     <row r="69" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="H69" s="3"/>
     </row>
     <row r="70" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="H73" s="3"/>
     </row>
     <row r="74" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="H76" s="3"/>
     </row>
     <row r="77" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="H77" s="3"/>
     </row>
     <row r="78" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="H78" s="3"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C79" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C80" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
     <mergeCell ref="E53:E54"/>
     <mergeCell ref="F53:F54"/>
     <mergeCell ref="E55:E56"/>
@@ -3381,6 +3359,33 @@
     <mergeCell ref="F49:F50"/>
     <mergeCell ref="E51:E52"/>
     <mergeCell ref="F51:F52"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:D54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3410,1089 +3415,1101 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="6" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="E27" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="B28" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D29" s="17"/>
+      <c r="D29" s="15"/>
     </row>
     <row r="30" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
+      <c r="D32" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B32" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="E32" s="6" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
       <c r="D33" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="C43" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
+      <c r="D43" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B43" s="17" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B45" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C45" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B45" s="17" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="17" t="s">
-        <v>248</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="2" t="s">
+      <c r="B49" s="15" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
+      <c r="C49" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="B47" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>252</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
       <c r="D50" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="17" t="s">
+      <c r="D53" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="15"/>
+      <c r="B54" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="D54" s="15"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="B55" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D53" s="17" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="17"/>
-      <c r="B54" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="D54" s="17"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>263</v>
-      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
       <c r="D56" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D65" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D53:D54"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B55:B56"/>
@@ -4507,18 +4524,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4526,6 +4531,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E2A70C0F482D004F81B909595C75DFA6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e14e4ad0a6f5f1a0ddcbf041a2a4a832">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="9ed5a28f-e285-4793-933e-f86572ea3e88" xmlns:ns3="6FDAA894-E433-443A-929C-6668B5175CA9" xmlns:ns4="a130c0bc-081d-4a7d-8c4b-0d956631a56e" xmlns:ns5="6fdaa894-e433-443a-929c-6668b5175ca9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f3fa50635c17e9cfabaeee8fe605afa8" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4730,15 +4744,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4753,6 +4758,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{211F509A-75D2-471F-BE44-DEEBD2FE04CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28D2A50F-394A-4741-95EF-7EE6194A4F57}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4770,14 +4783,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{211F509A-75D2-471F-BE44-DEEBD2FE04CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Removed old txCache files, add new ones
</commit_message>
<xml_diff>
--- a/mapping/Mappings.xlsx
+++ b/mapping/Mappings.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EC77D7-171C-45D8-AA66-53B482D210A6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5143B2-2156-404E-ACBF-DC086B45A293}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" activeTab="2" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
   </bookViews>
   <sheets>
     <sheet name="RR" sheetId="1" r:id="rId1"/>
     <sheet name="eICR" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_ftn1" localSheetId="2">Sheet1!#REF!</definedName>
+    <definedName name="_ftnref1" localSheetId="2">Sheet1!$A$2</definedName>
+  </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="405">
   <si>
     <t>Date and time of eICR Receipt</t>
   </si>
@@ -73,6 +78,9 @@
     <t>CD</t>
   </si>
   <si>
+    <t>eICR CDA Document ID</t>
+  </si>
+  <si>
     <t>Received eICR Information/eICR External Document Reference/id</t>
   </si>
   <si>
@@ -1105,9 +1113,6 @@
     <t>Observation[eicr-occupationhistory]</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>eICR Document ID</t>
   </si>
   <si>
@@ -1127,13 +1132,133 @@
   </si>
   <si>
     <t>action.documentation.extension-rr-priority</t>
+  </si>
+  <si>
+    <t>Pregnancy Observation</t>
+  </si>
+  <si>
+    <t>Composition[eicr-composition].section[Social History Section].entry</t>
+  </si>
+  <si>
+    <t>Observation[pregnancy-status]</t>
+  </si>
+  <si>
+    <t>Composition[eicr-composition].section[History of Present Illness]</t>
+  </si>
+  <si>
+    <t>Composition[eicr-composition].section[Reason for Visit]</t>
+  </si>
+  <si>
+    <t>Composition[eicr-composition].section[Problem Section]</t>
+  </si>
+  <si>
+    <t>Observation[us-core-condition]</t>
+  </si>
+  <si>
+    <t>RR Location</t>
+  </si>
+  <si>
+    <t>eICR Location</t>
+  </si>
+  <si>
+    <t>eICR CDA Document setId</t>
+  </si>
+  <si>
+    <t>eICR CDA Document versionNumber</t>
+  </si>
+  <si>
+    <t>Name of eICR file (e.g. "specific_eicr.xml")</t>
+  </si>
+  <si>
+    <t>Not sure if this will be located in the RCKMS output or not</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/guardian</t>
+  </si>
+  <si>
+    <t>This is contained in recordTarget, so if there is a guardian specified, then copying the recordTarget will ensure the guardian is also represented in the RR</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/code[code="PHC1464"]</t>
+  </si>
+  <si>
+    <t>Manually Initiated eICR/code["PHC1464"]</t>
+  </si>
+  <si>
+    <t>eICR External Document Reference/id</t>
+  </si>
+  <si>
+    <t>eICR External Document Reference/setId</t>
+  </si>
+  <si>
+    <t>eICR External Document Reference/versionNumber</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/setId</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/versionNumber</t>
+  </si>
+  <si>
+    <t>Copy entire recordTarget</t>
+  </si>
+  <si>
+    <t>Copy entire componentOf/encompassingEncounter</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/informationRecipient[@typeCode="PRCP"]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/responsibleParty/assignedEntity/address</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/responsibleParty/assignedEntity/telecom["mailto:"]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/responsibleParty/assignedEntity/telecom["fax:"]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/responsibleParty/assignedEntity/telecom["tel:"]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/responsibleParty/assignedEntity/assignedPerson/name</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/responsibleParty/assignedEntity/id</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/responsibleParty/assignedEntity/representedOrganization/name</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/informationRecipient[@typeCode="PRCP"]/intendedRecipient/addr</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/informationRecipient[@typeCode="PRCP"]/intendedRecipient/id</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/informationRecipient[@typeCode="PRCP"]/intendedRecipient/telecom["tel:"]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/informationRecipient[@typeCode="PRCP"]/intendedRecipient/telecom["mailto:"]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/informationRecipient[@typeCode="PRCP"]/intendedRecipient/informationRecipient/name</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/informationRecipient[@typeCode="PRCP"]/intendedRecipient/receivedOrganization/name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1159,6 +1284,28 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1196,7 +1343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1241,6 +1388,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1559,11 +1725,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2E64F1-05B1-4B7F-9A17-F737E551CA1E}">
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="77.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1582,31 +1748,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1639,13 +1805,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F3" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>287</v>
       </c>
       <c r="H3" s="3"/>
     </row>
@@ -1663,13 +1829,13 @@
         <v>7</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H4" s="3"/>
     </row>
@@ -1687,13 +1853,13 @@
         <v>12</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H5" s="3"/>
     </row>
@@ -1705,19 +1871,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H6" s="3"/>
     </row>
@@ -1729,15 +1895,15 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="10" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H7" s="3"/>
     </row>
@@ -1749,258 +1915,258 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="10" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>364</v>
@@ -2009,160 +2175,160 @@
     </row>
     <row r="19" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G25" s="14" t="s">
         <v>361</v>
@@ -2170,432 +2336,432 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="16"/>
@@ -2604,32 +2770,32 @@
     </row>
     <row r="45" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="16"/>
@@ -2638,32 +2804,32 @@
     </row>
     <row r="47" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A48" s="15"/>
       <c r="B48" s="15"/>
       <c r="C48" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D48" s="15"/>
       <c r="E48" s="17"/>
@@ -2672,32 +2838,32 @@
     </row>
     <row r="49" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D50" s="15"/>
       <c r="E50" s="16"/>
@@ -2705,32 +2871,32 @@
     </row>
     <row r="51" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
       <c r="C52" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="16"/>
@@ -2738,32 +2904,32 @@
     </row>
     <row r="53" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
       <c r="C54" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="16"/>
@@ -2771,32 +2937,32 @@
     </row>
     <row r="55" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="16"/>
@@ -2804,65 +2970,65 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H57" s="3"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H58" s="3"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>363</v>
@@ -2874,477 +3040,477 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H63" s="3"/>
     </row>
     <row r="64" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H64" s="3"/>
     </row>
     <row r="65" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H65" s="3"/>
     </row>
     <row r="66" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H66" s="3"/>
     </row>
     <row r="67" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H67" s="3"/>
     </row>
     <row r="68" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H68" s="3"/>
     </row>
     <row r="69" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H69" s="3"/>
     </row>
     <row r="70" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F71" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="G71" s="10" t="s">
         <v>327</v>
-      </c>
-      <c r="G71" s="10" t="s">
-        <v>326</v>
       </c>
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H73" s="3"/>
     </row>
     <row r="74" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H76" s="3"/>
     </row>
     <row r="77" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H77" s="3"/>
     </row>
     <row r="78" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H78" s="3"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C79" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C80" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G80" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="I80" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="I80" s="4" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3397,10 +3563,10 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3415,527 +3581,527 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -3943,361 +4109,388 @@
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D29" s="15"/>
     </row>
     <row r="30" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>219</v>
+        <v>365</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="C41" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="D42" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C47" s="15"/>
       <c r="D47" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="15"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
       <c r="D48" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -4305,73 +4498,73 @@
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
       <c r="D50" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="15"/>
       <c r="B54" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D54" s="15"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -4379,125 +4572,127 @@
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
       <c r="D56" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D65" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C32:C33"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
@@ -4506,10 +4701,8 @@
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D53:D54"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B55:B56"/>
@@ -4525,6 +4718,408 @@
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="A53:A54"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256CA3A7-5EF5-4FDD-8423-35F2A7AC76DA}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>372</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>387</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>388</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>392</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>394</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>395</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="26"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add back eicr-condition, update places used
</commit_message>
<xml_diff>
--- a/mapping/Mappings.xlsx
+++ b/mapping/Mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5143B2-2156-404E-ACBF-DC086B45A293}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACB5F96-5963-4D77-89C6-19C361550A93}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" activeTab="2" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" activeTab="1" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
   </bookViews>
   <sheets>
     <sheet name="RR" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="409">
   <si>
     <t>Date and time of eICR Receipt</t>
   </si>
@@ -1152,9 +1152,6 @@
     <t>Composition[eicr-composition].section[Problem Section]</t>
   </si>
   <si>
-    <t>Observation[us-core-condition]</t>
-  </si>
-  <si>
     <t>RR Location</t>
   </si>
   <si>
@@ -1252,6 +1249,21 @@
   </si>
   <si>
     <t>ClinicalDocument/informationRecipient[@typeCode="PRCP"]/intendedRecipient/receivedOrganization/name</t>
+  </si>
+  <si>
+    <t>Encounter[eicr-encounter]</t>
+  </si>
+  <si>
+    <t>Composition[eicr-composition].encounter</t>
+  </si>
+  <si>
+    <t>period.start</t>
+  </si>
+  <si>
+    <t>period.end</t>
+  </si>
+  <si>
+    <t>Observation[eicr-condition]</t>
   </si>
 </sst>
 </file>
@@ -1331,7 +1343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1339,11 +1351,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1390,23 +1417,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3562,11 +3597,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1E071C-8572-48FD-94ED-9BC2BF0CD944}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3575,7 +3610,9 @@
     <col min="2" max="2" width="41.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="44" style="4" customWidth="1"/>
+    <col min="5" max="5" width="44" style="4" customWidth="1"/>
+    <col min="6" max="6" width="53.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44" style="4" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -4298,6 +4335,15 @@
         <v>188</v>
       </c>
       <c r="D35" s="5"/>
+      <c r="E35" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
@@ -4312,6 +4358,15 @@
       <c r="D36" s="2" t="s">
         <v>226</v>
       </c>
+      <c r="E36" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
@@ -4326,6 +4381,15 @@
       <c r="D37" s="2" t="s">
         <v>228</v>
       </c>
+      <c r="E37" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
@@ -4340,6 +4404,15 @@
       <c r="D38" s="2" t="s">
         <v>228</v>
       </c>
+      <c r="E38" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
@@ -4398,7 +4471,7 @@
         <v>370</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>371</v>
+        <v>408</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -4727,397 +4800,427 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256CA3A7-5EF5-4FDD-8423-35F2A7AC76DA}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:D33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="29.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="D2" s="24"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
         <v>373</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>372</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" s="24" t="s">
+      <c r="B3" s="26" t="s">
+        <v>386</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="D3" s="24"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
         <v>374</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B4" s="26" t="s">
         <v>387</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C4" s="27" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="D6" s="24"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="D7" s="24"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="D10" s="24"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="D11" s="24"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="26" t="s">
         <v>375</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="C12" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="24"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="D15" s="24"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="D16" s="24"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D17" s="24" t="s">
         <v>388</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>386</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>386</v>
-      </c>
-      <c r="D5" s="22" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D18" s="24"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D20" s="24"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D21" s="24"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D22" s="24"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D23" s="24"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D24" s="24"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D25" s="24"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D26" s="24"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="D27" s="24"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="C28" s="30" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>386</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>386</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>386</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>386</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>386</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>386</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>376</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>381</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>382</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>379</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>379</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>379</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>379</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>378</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>378</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>378</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>378</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>378</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>378</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>378</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>378</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>378</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>378</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>378</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>392</v>
-      </c>
-      <c r="C27" s="26" t="s">
+      <c r="D28" s="24"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>401</v>
+      </c>
+      <c r="D29" s="24"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="C30" s="30" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" s="19" t="s">
+      <c r="D30" s="24"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>402</v>
+      </c>
+      <c r="D31" s="24"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="26" t="s">
         <v>394</v>
       </c>
-      <c r="C29" s="26" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30" s="19" t="s">
+      <c r="C32" s="30" t="s">
+        <v>400</v>
+      </c>
+      <c r="D32" s="24"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="26" t="s">
         <v>397</v>
       </c>
-      <c r="C30" s="26" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>396</v>
-      </c>
-      <c r="C31" s="26" t="s">
+      <c r="C33" s="30" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>395</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>398</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C34" s="26"/>
+      <c r="D33" s="24"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Formatting updates, renamed extension, etc.
</commit_message>
<xml_diff>
--- a/mapping/Mappings.xlsx
+++ b/mapping/Mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACB5F96-5963-4D77-89C6-19C361550A93}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE22936D-ADC6-4614-BF19-0FA4A763DB99}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" activeTab="1" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="415">
   <si>
     <t>Date and time of eICR Receipt</t>
   </si>
@@ -1149,9 +1149,6 @@
     <t>Composition[eicr-composition].section[Reason for Visit]</t>
   </si>
   <si>
-    <t>Composition[eicr-composition].section[Problem Section]</t>
-  </si>
-  <si>
     <t>RR Location</t>
   </si>
   <si>
@@ -1264,6 +1261,27 @@
   </si>
   <si>
     <t>Observation[eicr-condition]</t>
+  </si>
+  <si>
+    <t>Composition[eicr-composition].section[Problem Section].entry</t>
+  </si>
+  <si>
+    <t>onset.start</t>
+  </si>
+  <si>
+    <t>Observation[eicr-travel-history]</t>
+  </si>
+  <si>
+    <t>effective[x]</t>
+  </si>
+  <si>
+    <t>component.valueCodeableConcept.text</t>
+  </si>
+  <si>
+    <t>component.valueCodeableConcept.coding</t>
+  </si>
+  <si>
+    <t>component.valueCodeableConcept.coding.extension-eicr-travel-history-address</t>
   </si>
 </sst>
 </file>
@@ -3598,10 +3616,10 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F41" sqref="F41"/>
+      <selection pane="bottomRight" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3610,7 +3628,7 @@
     <col min="2" max="2" width="41.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44" style="4" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="53.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44" style="4" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="4"/>
@@ -4359,13 +4377,13 @@
         <v>226</v>
       </c>
       <c r="E36" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>405</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -4382,13 +4400,13 @@
         <v>228</v>
       </c>
       <c r="E37" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>405</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -4405,13 +4423,13 @@
         <v>228</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -4468,10 +4486,13 @@
         <v>179</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>370</v>
+        <v>408</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -4486,6 +4507,15 @@
       </c>
       <c r="D42" s="2" t="s">
         <v>179</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -4552,7 +4582,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
         <v>248</v>
       </c>
@@ -4566,7 +4596,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -4574,7 +4604,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>252</v>
       </c>
@@ -4588,7 +4618,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>254</v>
       </c>
@@ -4602,7 +4632,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
         <v>256</v>
       </c>
@@ -4616,7 +4646,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="15"/>
       <c r="B54" s="2" t="s">
         <v>245</v>
@@ -4626,7 +4656,7 @@
       </c>
       <c r="D54" s="15"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
         <v>260</v>
       </c>
@@ -4640,7 +4670,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
@@ -4648,7 +4678,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>262</v>
       </c>
@@ -4662,7 +4692,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>265</v>
       </c>
@@ -4676,7 +4706,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>267</v>
       </c>
@@ -4690,7 +4720,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>270</v>
       </c>
@@ -4702,7 +4732,7 @@
       </c>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>271</v>
       </c>
@@ -4714,7 +4744,7 @@
       </c>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>274</v>
       </c>
@@ -4725,8 +4755,17 @@
         <v>276</v>
       </c>
       <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+      <c r="E62" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>277</v>
       </c>
@@ -4737,8 +4776,17 @@
         <v>278</v>
       </c>
       <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+      <c r="E63" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>279</v>
       </c>
@@ -4749,8 +4797,17 @@
         <v>280</v>
       </c>
       <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+      <c r="E64" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>281</v>
       </c>
@@ -4761,6 +4818,15 @@
         <v>282</v>
       </c>
       <c r="D65" s="2"/>
+      <c r="E65" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>414</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="26">
@@ -4818,10 +4884,10 @@
         <v>170</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>284</v>
@@ -4835,31 +4901,31 @@
         <v>131</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D4" s="24"/>
     </row>
@@ -4868,13 +4934,13 @@
         <v>19</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4882,10 +4948,10 @@
         <v>48</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D6" s="24"/>
     </row>
@@ -4894,10 +4960,10 @@
         <v>56</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D7" s="24"/>
     </row>
@@ -4906,10 +4972,10 @@
         <v>51</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D8" s="24"/>
     </row>
@@ -4918,10 +4984,10 @@
         <v>53</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D9" s="24"/>
     </row>
@@ -4930,10 +4996,10 @@
         <v>58</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D10" s="24"/>
     </row>
@@ -4942,10 +5008,10 @@
         <v>60</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D11" s="24"/>
     </row>
@@ -4954,7 +5020,7 @@
         <v>62</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>63</v>
@@ -4966,13 +5032,13 @@
         <v>68</v>
       </c>
       <c r="B13" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="C13" s="30" t="s">
         <v>380</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>381</v>
-      </c>
       <c r="D13" s="24" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
@@ -4980,13 +5046,13 @@
         <v>72</v>
       </c>
       <c r="B14" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D14" s="24" t="s">
         <v>378</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4994,10 +5060,10 @@
         <v>74</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D15" s="24"/>
     </row>
@@ -5006,10 +5072,10 @@
         <v>76</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D16" s="24"/>
     </row>
@@ -5018,13 +5084,13 @@
         <v>78</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -5032,10 +5098,10 @@
         <v>80</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D18" s="24"/>
     </row>
@@ -5044,10 +5110,10 @@
         <v>82</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D19" s="24"/>
     </row>
@@ -5056,10 +5122,10 @@
         <v>84</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D20" s="24"/>
     </row>
@@ -5068,10 +5134,10 @@
         <v>86</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D21" s="24"/>
     </row>
@@ -5080,10 +5146,10 @@
         <v>88</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D22" s="24"/>
     </row>
@@ -5092,10 +5158,10 @@
         <v>90</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D23" s="24"/>
     </row>
@@ -5104,10 +5170,10 @@
         <v>92</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D24" s="24"/>
     </row>
@@ -5116,10 +5182,10 @@
         <v>94</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D25" s="24"/>
     </row>
@@ -5128,10 +5194,10 @@
         <v>96</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D26" s="24"/>
     </row>
@@ -5140,10 +5206,10 @@
         <v>98</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D27" s="24"/>
     </row>
@@ -5152,10 +5218,10 @@
         <v>101</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D28" s="24"/>
     </row>
@@ -5164,10 +5230,10 @@
         <v>107</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D29" s="24"/>
     </row>
@@ -5176,10 +5242,10 @@
         <v>110</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D30" s="24"/>
     </row>
@@ -5188,10 +5254,10 @@
         <v>113</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D31" s="24"/>
     </row>
@@ -5200,10 +5266,10 @@
         <v>116</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D32" s="24"/>
     </row>
@@ -5212,10 +5278,10 @@
         <v>104</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D33" s="24"/>
     </row>

</xml_diff>

<commit_message>
Updated slicing in composition
</commit_message>
<xml_diff>
--- a/mapping/Mappings.xlsx
+++ b/mapping/Mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE22936D-ADC6-4614-BF19-0FA4A763DB99}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB759595-EB3B-4B76-A1A5-D190831EE027}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" activeTab="1" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="417">
   <si>
     <t>Date and time of eICR Receipt</t>
   </si>
@@ -1282,6 +1282,12 @@
   </si>
   <si>
     <t>component.valueCodeableConcept.coding.extension-eicr-travel-history-address</t>
+  </si>
+  <si>
+    <t>Compoition[eicr-composition].subject</t>
+  </si>
+  <si>
+    <t>deceasedDateTime</t>
   </si>
 </sst>
 </file>
@@ -3619,7 +3625,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E61" sqref="E61"/>
+      <selection pane="bottomRight" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -4731,6 +4737,15 @@
         <v>264</v>
       </c>
       <c r="D60" s="2"/>
+      <c r="E60" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">

</xml_diff>

<commit_message>
Update profiles page, labels in structure defintions
</commit_message>
<xml_diff>
--- a/mapping/Mappings.xlsx
+++ b/mapping/Mappings.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEB13C2-99DC-4B1E-8AEC-F7CBCE46CD0E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA7AF97-B5C6-4B49-859E-E7A6EB365904}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" activeTab="1" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12600" xr2:uid="{69CB834B-E9B6-4361-B34A-B68FB7F004FE}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{69CB834B-E9B6-4361-B34A-B68FB7F004FE}"/>
   </bookViews>
   <sheets>
     <sheet name="RR" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="396">
   <si>
     <t>Date and time of eICR Receipt</t>
   </si>
@@ -497,9 +497,6 @@
   </si>
   <si>
     <t>Reportability Response/custodian</t>
-  </si>
-  <si>
-    <t>Same as author</t>
   </si>
   <si>
     <t>Communication.sender</t>
@@ -1199,6 +1196,39 @@
   </si>
   <si>
     <t>ID of the eICR Document</t>
+  </si>
+  <si>
+    <t>StructureDefinition-extension-rr-determination-of-reportability-reason.html</t>
+  </si>
+  <si>
+    <t>StructureDefinition-extension-rr-determination-of-reportability-rule.html</t>
+  </si>
+  <si>
+    <t>StructureDefinition-extension-rr-determination-of-reportability.html</t>
+  </si>
+  <si>
+    <t>StructureDefinition-extension-rr-external-resource-type.html</t>
+  </si>
+  <si>
+    <t>StructureDefinition-extension-rr-manually-initiated-eicr.html</t>
+  </si>
+  <si>
+    <t>StructureDefinition-extension-eicr-travel-history-address.html</t>
+  </si>
+  <si>
+    <t>StructureDefinition-extension-eicr-manually-initiated-reason</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-composition-definitions.html#Composition.date</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-composition-definitions.html#Composition.id</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-composition-definitions.html#Composition.identifier</t>
+  </si>
+  <si>
+    <t>StructureDefinition-pregnancy-status.html#sd-26-structuredefinition-pregnancy-status</t>
   </si>
 </sst>
 </file>
@@ -1343,15 +1373,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1378,6 +1399,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1693,16 +1723,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2E64F1-05B1-4B7F-9A17-F737E551CA1E}">
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B78" sqref="B78"/>
+      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="D1" workbookViewId="1">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="77.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1714,13 +1744,12 @@
     <col min="5" max="5" width="35.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="21" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="77.140625" style="4"/>
+    <col min="8" max="16384" width="77.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>19</v>
@@ -1729,22 +1758,19 @@
         <v>20</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1757,7 +1783,7 @@
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1768,17 +1794,19 @@
         <v>5</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1789,17 +1817,19 @@
         <v>7</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E4" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="G4" s="3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1810,19 +1840,21 @@
         <v>9</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
@@ -1831,19 +1863,19 @@
         <v>11</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>196</v>
-      </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
@@ -1854,13 +1886,13 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
@@ -1871,11 +1903,11 @@
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1886,18 +1918,17 @@
         <v>16</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1908,18 +1939,17 @@
         <v>18</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E10" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>203</v>
-      </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1930,18 +1960,17 @@
         <v>22</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1952,18 +1981,17 @@
         <v>24</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -1974,18 +2002,17 @@
         <v>26</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -1996,18 +2023,17 @@
         <v>28</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
@@ -2018,17 +2044,19 @@
         <v>30</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
@@ -2039,13 +2067,13 @@
         <v>32</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -2060,13 +2088,13 @@
         <v>34</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G17" s="3"/>
     </row>
@@ -2081,13 +2109,13 @@
         <v>36</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -2102,13 +2130,13 @@
         <v>38</v>
       </c>
       <c r="D19" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>250</v>
-      </c>
       <c r="F19" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -2122,13 +2150,13 @@
         <v>40</v>
       </c>
       <c r="D20" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>250</v>
-      </c>
       <c r="F20" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -2142,13 +2170,13 @@
         <v>42</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>250</v>
-      </c>
       <c r="F21" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -2162,13 +2190,13 @@
         <v>44</v>
       </c>
       <c r="D22" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>250</v>
-      </c>
       <c r="F22" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -2182,13 +2210,13 @@
         <v>46</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>250</v>
-      </c>
       <c r="F23" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -2202,13 +2230,13 @@
         <v>48</v>
       </c>
       <c r="D24" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="F24" s="8" t="s">
         <v>250</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -2222,13 +2250,13 @@
         <v>50</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2242,13 +2270,13 @@
         <v>52</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -2262,17 +2290,17 @@
         <v>54</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
@@ -2283,15 +2311,17 @@
         <v>56</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="G28" s="3"/>
+        <v>214</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
@@ -2304,13 +2334,13 @@
         <v>58</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -2324,13 +2354,13 @@
         <v>60</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -2341,16 +2371,16 @@
         <v>15</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -2364,13 +2394,13 @@
         <v>63</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -2384,13 +2414,13 @@
         <v>65</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E33" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F33" s="9" t="s">
         <v>219</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>220</v>
       </c>
       <c r="G33" s="3"/>
     </row>
@@ -2405,13 +2435,13 @@
         <v>67</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G34" s="3"/>
     </row>
@@ -2426,13 +2456,13 @@
         <v>69</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -2446,13 +2476,13 @@
         <v>71</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G36" s="3"/>
     </row>
@@ -2467,13 +2497,13 @@
         <v>73</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G37" s="3"/>
     </row>
@@ -2488,13 +2518,13 @@
         <v>75</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G38" s="3"/>
     </row>
@@ -2509,13 +2539,13 @@
         <v>77</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -2529,13 +2559,13 @@
         <v>79</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G40" s="3"/>
     </row>
@@ -2550,13 +2580,13 @@
         <v>81</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G41" s="3"/>
     </row>
@@ -2571,222 +2601,222 @@
         <v>83</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="E43" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="E43" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>226</v>
+      <c r="F43" s="29" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="17"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="29"/>
     </row>
     <row r="45" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="E45" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="E45" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>228</v>
+      <c r="F45" s="29" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
       <c r="C46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="17"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="29"/>
     </row>
     <row r="47" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="E47" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="E47" s="17" t="s">
-        <v>257</v>
-      </c>
       <c r="F47" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A48" s="15"/>
-      <c r="B48" s="15"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="30"/>
       <c r="C48" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
       <c r="F48" s="11"/>
     </row>
-    <row r="49" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A49" s="15" t="s">
+    <row r="49" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A49" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="D49" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="E49" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="E49" s="16" t="s">
-        <v>248</v>
-      </c>
       <c r="F49" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
       <c r="C50" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-    </row>
-    <row r="51" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A51" s="15" t="s">
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+    </row>
+    <row r="51" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A51" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="E51" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="E51" s="16" t="s">
-        <v>248</v>
-      </c>
       <c r="F51" s="8" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="15"/>
-      <c r="B52" s="15"/>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="30"/>
+      <c r="B52" s="30"/>
       <c r="C52" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-    </row>
-    <row r="53" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+    </row>
+    <row r="53" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A53" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="E53" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="E53" s="16" t="s">
-        <v>248</v>
-      </c>
       <c r="F53" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A54" s="15"/>
-      <c r="B54" s="15"/>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A54" s="30"/>
+      <c r="B54" s="30"/>
       <c r="C54" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-    </row>
-    <row r="55" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A55" s="15" t="s">
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+    </row>
+    <row r="55" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A55" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="E55" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="E55" s="16" t="s">
-        <v>248</v>
-      </c>
       <c r="F55" s="8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="15"/>
-      <c r="B56" s="15"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="30"/>
+      <c r="B56" s="30"/>
       <c r="C56" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>105</v>
       </c>
@@ -2797,17 +2827,17 @@
         <v>106</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>107</v>
       </c>
@@ -2818,17 +2848,17 @@
         <v>108</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>109</v>
       </c>
@@ -2839,17 +2869,16 @@
         <v>110</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="H59" s="3"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>111</v>
       </c>
@@ -2860,17 +2889,17 @@
         <v>113</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>114</v>
       </c>
@@ -2881,17 +2910,17 @@
         <v>115</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G61" s="3"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>116</v>
       </c>
@@ -2902,17 +2931,17 @@
         <v>117</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>118</v>
       </c>
@@ -2923,17 +2952,17 @@
         <v>119</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>120</v>
       </c>
@@ -2944,17 +2973,17 @@
         <v>121</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>122</v>
       </c>
@@ -2965,17 +2994,17 @@
         <v>123</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>124</v>
       </c>
@@ -2986,17 +3015,17 @@
         <v>125</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E66" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="F66" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="F66" s="9" t="s">
-        <v>236</v>
-      </c>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>126</v>
       </c>
@@ -3007,17 +3036,17 @@
         <v>127</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>128</v>
       </c>
@@ -3028,17 +3057,17 @@
         <v>129</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G68" s="3"/>
     </row>
-    <row r="69" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>130</v>
       </c>
@@ -3049,17 +3078,17 @@
         <v>131</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G69" s="3"/>
     </row>
-    <row r="70" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>132</v>
       </c>
@@ -3070,17 +3099,17 @@
         <v>133</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G70" s="3"/>
     </row>
-    <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>134</v>
       </c>
@@ -3091,17 +3120,17 @@
         <v>135</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G71" s="3"/>
     </row>
-    <row r="72" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>136</v>
       </c>
@@ -3112,17 +3141,17 @@
         <v>137</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G72" s="3"/>
     </row>
-    <row r="73" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>138</v>
       </c>
@@ -3133,17 +3162,17 @@
         <v>139</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G73" s="3"/>
     </row>
-    <row r="74" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>140</v>
       </c>
@@ -3154,17 +3183,17 @@
         <v>141</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G74" s="3"/>
     </row>
-    <row r="75" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>142</v>
       </c>
@@ -3175,17 +3204,17 @@
         <v>143</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G75" s="3"/>
     </row>
-    <row r="76" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>144</v>
       </c>
@@ -3196,17 +3225,17 @@
         <v>145</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G76" s="3"/>
     </row>
-    <row r="77" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>146</v>
       </c>
@@ -3217,17 +3246,17 @@
         <v>147</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G77" s="3"/>
     </row>
-    <row r="78" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>148</v>
       </c>
@@ -3238,17 +3267,17 @@
         <v>149</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G78" s="3"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C79" s="3" t="s">
         <v>150</v>
       </c>
@@ -3256,19 +3285,36 @@
         <v>151</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C80" s="3" t="s">
         <v>152</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="H80" s="4" t="s">
         <v>153</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
     <mergeCell ref="D53:D54"/>
     <mergeCell ref="E53:E54"/>
     <mergeCell ref="D55:D56"/>
@@ -3279,26 +3325,6 @@
     <mergeCell ref="E49:E50"/>
     <mergeCell ref="D51:D52"/>
     <mergeCell ref="E51:E52"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3307,29 +3333,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1E071C-8572-48FD-94ED-9BC2BF0CD944}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E55" sqref="E55"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="1">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="73.5703125" style="4" customWidth="1"/>
-    <col min="4" max="5" width="77.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="44" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="7" max="7" width="69.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>19</v>
@@ -3338,1088 +3368,1109 @@
         <v>20</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>157</v>
-      </c>
       <c r="C2" s="14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>382</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>367</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="B15" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>73</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>75</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>77</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>63</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>60</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>82</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>83</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>67</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>352</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>80</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>81</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>71</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>79</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B30" s="14" t="s">
-        <v>352</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="B31" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>275</v>
-      </c>
       <c r="F31" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>312</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D34" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>312</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B36" s="14" t="s">
-        <v>170</v>
-      </c>
       <c r="C36" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="B37" s="14" t="s">
-        <v>172</v>
-      </c>
       <c r="C37" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E38" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>315</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B39" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="C39" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="C39" s="14" t="s">
-        <v>342</v>
-      </c>
       <c r="D39" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D42" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>325</v>
-      </c>
       <c r="F42" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B43" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="C43" s="14" t="s">
-        <v>348</v>
-      </c>
       <c r="E43" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C46" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>182</v>
-      </c>
       <c r="D46" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C48" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="D48" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="C48" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="C50" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="C50" s="14" t="s">
+      <c r="B51" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="C51" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="C51" s="14" t="s">
+      <c r="B52" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>353</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="F51" s="4" t="s">
+      <c r="D52" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="C52" s="14" t="s">
+      <c r="B53" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C53" s="14" t="s">
         <v>354</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="F52" s="4" t="s">
+      <c r="D53" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="F53" s="4" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+    <row r="54" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="C53" s="14" t="s">
+      <c r="B54" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C54" s="14" t="s">
         <v>355</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="F53" s="4" t="s">
+      <c r="D54" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" s="4" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C55" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="E55" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="F55" s="4" t="s">
+      <c r="C56" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>379</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -4439,421 +4490,421 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="29.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>278</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="27" t="s">
+      <c r="B3" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>289</v>
       </c>
-      <c r="D2" s="24"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C4" s="24" t="s">
         <v>290</v>
       </c>
-      <c r="D3" s="24"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D10" s="21"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="23" t="s">
         <v>281</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="C12" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>291</v>
-      </c>
-      <c r="D4" s="24"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="D5" s="24" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D18" s="21"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D22" s="21"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D23" s="21"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D24" s="21"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D25" s="21"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>304</v>
+      </c>
+      <c r="D27" s="21"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="C28" s="27" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="D6" s="24"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="D7" s="24"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="D8" s="24"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="D9" s="24"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="D10" s="24"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="D11" s="24"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>282</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="24"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>287</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>288</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="D15" s="24"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="D16" s="24"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="D18" s="24"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="D19" s="24"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="D20" s="24"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="D21" s="24"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="D22" s="24"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="D23" s="24"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="D24" s="24"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="D25" s="24"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="D26" s="24"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="C27" s="30" t="s">
+      <c r="D28" s="21"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>307</v>
+      </c>
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="C30" s="27" t="s">
         <v>305</v>
       </c>
-      <c r="D27" s="24"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>297</v>
-      </c>
-      <c r="D28" s="24"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="26" t="s">
+      <c r="D30" s="21"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>301</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="C29" s="30" t="s">
-        <v>308</v>
-      </c>
-      <c r="D29" s="24"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="26" t="s">
+      <c r="C32" s="27" t="s">
+        <v>306</v>
+      </c>
+      <c r="D32" s="21"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="C30" s="30" t="s">
-        <v>306</v>
-      </c>
-      <c r="D30" s="24"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>302</v>
-      </c>
-      <c r="C31" s="30" t="s">
+      <c r="C33" s="27" t="s">
         <v>309</v>
       </c>
-      <c r="D31" s="24"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>301</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>307</v>
-      </c>
-      <c r="D32" s="24"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>304</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>310</v>
-      </c>
-      <c r="D33" s="24"/>
+      <c r="D33" s="21"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C34" s="21"/>
+      <c r="C34" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4862,12 +4913,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LCG_x0020_Document_x0020_Workflow xmlns="6FDAA894-E433-443A-929C-6668B5175CA9">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </LCG_x0020_Document_x0020_Workflow>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5076,22 +5131,30 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LCG_x0020_Document_x0020_Workflow xmlns="6FDAA894-E433-443A-929C-6668B5175CA9">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </LCG_x0020_Document_x0020_Workflow>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{211F509A-75D2-471F-BE44-DEEBD2FE04CC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B0C849C-1E0C-4B3D-9203-5FFDB8062BA1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="6fdaa894-e433-443a-929c-6668b5175ca9"/>
+    <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6FDAA894-E433-443A-929C-6668B5175CA9"/>
+    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5119,21 +5182,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B0C849C-1E0C-4B3D-9203-5FFDB8062BA1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{211F509A-75D2-471F-BE44-DEEBD2FE04CC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="6fdaa894-e433-443a-929c-6668b5175ca9"/>
-    <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6FDAA894-E433-443A-929C-6668B5175CA9"/>
-    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Various changes, bug fixes etc.
</commit_message>
<xml_diff>
--- a/mapping/Mappings.xlsx
+++ b/mapping/Mappings.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA7AF97-B5C6-4B49-859E-E7A6EB365904}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D3DDD7-222C-4788-98EB-50E683F715F5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{69CB834B-E9B6-4361-B34A-B68FB7F004FE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="7665" activeTab="1" xr2:uid="{69CB834B-E9B6-4361-B34A-B68FB7F004FE}"/>
   </bookViews>
   <sheets>
     <sheet name="RR" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="485">
   <si>
     <t>Date and time of eICR Receipt</t>
   </si>
@@ -694,9 +694,6 @@
     <t>component[code="RRVS31"].valueCode</t>
   </si>
   <si>
-    <t>Patient[us-core-patient]</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
@@ -824,9 +821,6 @@
   </si>
   <si>
     <t>Encounter[eicr-encounter].participant[type="ATND"].PractitionerRole[ecr-practitionerrole].practitioner</t>
-  </si>
-  <si>
-    <t>Encounter[eicr-encounter].participant[type="ATND"].PractitionerRole[ecr-practitionerrole].location</t>
   </si>
   <si>
     <t>Location(eicr-location)</t>
@@ -1213,22 +1207,295 @@
     <t>StructureDefinition-extension-rr-manually-initiated-eicr.html</t>
   </si>
   <si>
-    <t>StructureDefinition-extension-eicr-travel-history-address.html</t>
-  </si>
-  <si>
-    <t>StructureDefinition-extension-eicr-manually-initiated-reason</t>
-  </si>
-  <si>
     <t>StructureDefinition-eicr-composition-definitions.html#Composition.date</t>
   </si>
   <si>
     <t>StructureDefinition-eicr-composition-definitions.html#Composition.id</t>
   </si>
   <si>
-    <t>StructureDefinition-eicr-composition-definitions.html#Composition.identifier</t>
-  </si>
-  <si>
-    <t>StructureDefinition-pregnancy-status.html#sd-26-structuredefinition-pregnancy-status</t>
+    <t>StructureDefinition-eicr-location-definitions.html#Location.name</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.identifier</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.address</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.name</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.telecom</t>
+  </si>
+  <si>
+    <t>Encounter[eicr-encounter].participant[type="ATND"]</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-location-definitions.html#Location.identifier</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-location-definitions.html#Location.type</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-location-definitions.html#Location.address</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-location-definitions.html#Location.telecom</t>
+  </si>
+  <si>
+    <t>Patient[ecr-patient]</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.extension:race</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.extension:ethnicity</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.identifier</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.name</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.address</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.birthdate</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.telecom</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.extension:birthsex</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.communication.language</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.deceased[x]</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.contact.name</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.contact.telecom</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-encounter-definitions.html#Encounter.period</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-composition-definitions.html#Composition.section:sliceHistoryOfPresentIllnessSection.text</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-composition-definitions.html#Composition.section:sliceReasonForVisitSection.text</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-condition-definitions.html#Condition.onset[x]</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-condition-definitions.html#Condition.code</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-procedurerequest-definitions.html#ProcedureRequest.code</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-composition-definitions.html#Composition.section:slicePlanOfTreatmentSection.entry:sliceEICRProcedureRequest.extension:sliceTriggerEICRProcedureRequest</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-travel-history-definitions.html#Observation.effective[x]</t>
+  </si>
+  <si>
+    <t>https://www.hl7.org/fhir/us/core/StructureDefinition-us-core-observationresults-definitions.html#Observation.code</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-composition-definitions.html#Composition.section:sliceResultsSection.entry:sliceUSCoreObservationResults.extension:sliceTriggerUSCoreObservationResults</t>
+  </si>
+  <si>
+    <t>StructureDefinition-us-core-observationresults-definitions.html#Observation.identifier</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-composition-definitions.html#Composition.section:sliceProblemSection.entry:sliceEICRCondition.extension:sliceTriggerCondition</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-condition-definitions.html#Condition.assertedDate</t>
+  </si>
+  <si>
+    <t>https://www.hl7.org/fhir/us/core/StructureDefinition-us-core-medicationstatement-definitions.html#MedicationStatement.medication[x]</t>
+  </si>
+  <si>
+    <t>https://www.hl7.org/fhir/us/core/StructureDefinition-us-core-immunization.html</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-travel-history-definitions.html#Observation.component.valueCodeableConcept:valueCodeableConcept.text</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-travel-history-definitions.html#Observation.component.valueCodeableConcept:valueCodeableConcept.coding</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-travel-history-definitions.html#Observation.component.valueCodeableConcept:valueCodeableConcept.extension:travelHistoryAddress</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-composition-definitions.html#Composition.extension:extensionEICRManuallyInitiatedReason</t>
+  </si>
+  <si>
+    <t>StructureDefinition-eicr-occupationhistory-definitions.html#Observation</t>
+  </si>
+  <si>
+    <t>StructureDefinition-pregnancy-status-definitions.html#Observation</t>
+  </si>
+  <si>
+    <t>[name](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.name)</t>
+  </si>
+  <si>
+    <t>[telecom[system="phone"]](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.telecom)</t>
+  </si>
+  <si>
+    <t>[telecom[system="fax"]](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.telecom)</t>
+  </si>
+  <si>
+    <t>[telecom[system="email"]](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.telecom)</t>
+  </si>
+  <si>
+    <t>[name](StructureDefinition-eicr-location-definitions.html#Location.name)</t>
+  </si>
+  <si>
+    <t>[address](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.address)</t>
+  </si>
+  <si>
+    <t>[identifier](StructureDefinition-eicr-location-definitions.html#Location.identifier)</t>
+  </si>
+  <si>
+    <t>[type](StructureDefinition-eicr-location-definitions.html#Location.type)</t>
+  </si>
+  <si>
+    <t>[telecom[system="phone"]](StructureDefinition-eicr-location-definitions.html#Location.telecom)</t>
+  </si>
+  <si>
+    <t>[telecom[system="fax"]](StructureDefinition-eicr-location-definitions.html#Location.telecom)</t>
+  </si>
+  <si>
+    <t>[address](StructureDefinition-eicr-location-definitions.html#Location.address)</t>
+  </si>
+  <si>
+    <t>[identifier](StructureDefinition-ecr-patient-definitions.html#Patient.identifier)</t>
+  </si>
+  <si>
+    <t>[name](StructureDefinition-ecr-patient-definitions.html#Patient.name)</t>
+  </si>
+  <si>
+    <t>[telecom[system="phone"]](StructureDefinition-ecr-patient-definitions.html#Patient.telecom)</t>
+  </si>
+  <si>
+    <t>[telecom[system="email"]](StructureDefinition-ecr-patient-definitions.html#Patient.telecom)</t>
+  </si>
+  <si>
+    <t>[contact.name](StructureDefinition-ecr-patient-definitions.html#Patient.contact.name)</t>
+  </si>
+  <si>
+    <t>[contact.telecom[system="phone"]](StructureDefinition-ecr-patient-definitions.html#Patient.contact.telecom)</t>
+  </si>
+  <si>
+    <t>[contact.telecom[system="email"]](StructureDefinition-ecr-patient-definitions.html#Patient.contact.telecom)</t>
+  </si>
+  <si>
+    <t>[address](StructureDefinition-ecr-patient-definitions.html#Patient.address)</t>
+  </si>
+  <si>
+    <t>[birthdate](StructureDefinition-ecr-patient-definitions.html#Patient.birthdate)</t>
+  </si>
+  <si>
+    <t>[us-core-birthsex](StructureDefinition-ecr-patient-definitions.html#Patient.extension:birthsex)</t>
+  </si>
+  <si>
+    <t>[us-core-race](StructureDefinition-ecr-patient-definitions.html#Patient.extension:race)</t>
+  </si>
+  <si>
+    <t>[us-core-ethnicity](StructureDefinition-ecr-patient-definitions.html#Patient.extension:ethnicity)</t>
+  </si>
+  <si>
+    <t>[communication.language](StructureDefinition-ecr-patient-definitions.html#Patient.communication.language)</t>
+  </si>
+  <si>
+    <t>[valueCodeableConcept](StructureDefinition-eicr-occupationhistory-definitions.html#Observation)</t>
+  </si>
+  <si>
+    <t>[valueCodeableConcept](StructureDefinition-pregnancy-status-definitions.html#Observation)</t>
+  </si>
+  <si>
+    <t>[period.start](StructureDefinition-eicr-encounter-definitions.html#Encounter.period)</t>
+  </si>
+  <si>
+    <t>[period.end](StructureDefinition-eicr-encounter-definitions.html#Encounter.period)</t>
+  </si>
+  <si>
+    <t>[text](StructureDefinition-eicr-composition-definitions.html#Composition.section:sliceHistoryOfPresentIllnessSection.text)</t>
+  </si>
+  <si>
+    <t>[text](StructureDefinition-eicr-composition-definitions.html#Composition.section:sliceReasonForVisitSection.text)</t>
+  </si>
+  <si>
+    <t>[onset.start](StructureDefinition-eicr-condition-definitions.html#Condition.onset[x])</t>
+  </si>
+  <si>
+    <t>[code](StructureDefinition-eicr-condition-definitions.html#Condition.code)</t>
+  </si>
+  <si>
+    <t>[code](StructureDefinition-eicr-procedurerequest-definitions.html#ProcedureRequest.code)</t>
+  </si>
+  <si>
+    <t>[extension-eicr-trigger-code-flag](StructureDefinition-eicr-composition-definitions.html#Composition.section:slicePlanOfTreatmentSection.entry:sliceEICRProcedureRequest.extension:sliceTriggerEICRProcedureRequest)</t>
+  </si>
+  <si>
+    <t>[code and/or valueCodeableConcept](https://www.hl7.org/fhir/us/core/StructureDefinition-us-core-observationresults-definitions.html#Observation.code)</t>
+  </si>
+  <si>
+    <t>[extension-eicr-trigger-code-flag](StructureDefinition-eicr-composition-definitions.html#Composition.section:sliceResultsSection.entry:sliceUSCoreObservationResults.extension:sliceTriggerUSCoreObservationResults)</t>
+  </si>
+  <si>
+    <t>[identifier](StructureDefinition-us-core-observationresults-definitions.html#Observation.identifier)</t>
+  </si>
+  <si>
+    <t>[extension-eicr-trigger-code-flag](StructureDefinition-eicr-composition-definitions.html#Composition.section:sliceProblemSection.entry:sliceEICRCondition.extension:sliceTriggerCondition)</t>
+  </si>
+  <si>
+    <t>[assertedDate](StructureDefinition-eicr-condition-definitions.html#Condition.assertedDate)</t>
+  </si>
+  <si>
+    <t>[medication[x]](https://www.hl7.org/fhir/us/core/StructureDefinition-us-core-medicationstatement-definitions.html#MedicationStatement.medication[x])</t>
+  </si>
+  <si>
+    <t>[deceasedDateTime](StructureDefinition-ecr-patient-definitions.html#Patient.deceased[x])</t>
+  </si>
+  <si>
+    <t>[](https://www.hl7.org/fhir/us/core/StructureDefinition-us-core-immunization.html)</t>
+  </si>
+  <si>
+    <t>[effective[x]](StructureDefinition-eicr-travel-history-definitions.html#Observation.effective[x])</t>
+  </si>
+  <si>
+    <t>[component.valueCodeableConcept.text](StructureDefinition-eicr-travel-history-definitions.html#Observation.component.valueCodeableConcept:valueCodeableConcept.text)</t>
+  </si>
+  <si>
+    <t>[component.valueCodeableConcept.coding](StructureDefinition-eicr-travel-history-definitions.html#Observation.component.valueCodeableConcept:valueCodeableConcept.coding)</t>
+  </si>
+  <si>
+    <t>[component.valueCodeableConcept.coding.extension-eicr-travel-history-address](StructureDefinition-eicr-travel-history-definitions.html#Observation.component.valueCodeableConcept:valueCodeableConcept.extension:travelHistoryAddress)</t>
+  </si>
+  <si>
+    <t>[extension-eicr-manually-initiated-reason](StructureDefinition-eicr-composition-definitions.html#Composition.extension:extensionEICRManuallyInitiatedReason)</t>
+  </si>
+  <si>
+    <t>[extension-eicr-manually-initiated-reason.valueString](StructureDefinition-eicr-composition-definitions.html#Composition.extension:extensionEICRManuallyInitiatedReason)</t>
+  </si>
+  <si>
+    <t>[date](StructureDefinition-eicr-composition-definitions.html#Composition.date)</t>
+  </si>
+  <si>
+    <t>[id](StructureDefinition-eicr-composition-definitions.html#Composition.id)</t>
+  </si>
+  <si>
+    <t>[identifier](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.identifier)</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1369,6 +1636,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1726,13 +1996,13 @@
   <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
     <sheetView topLeftCell="D1" workbookViewId="1">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="77.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1758,13 +2028,13 @@
         <v>20</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>205</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>212</v>
@@ -1794,7 +2064,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>197</v>
@@ -1803,7 +2073,7 @@
         <v>196</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="36" x14ac:dyDescent="0.2">
@@ -1817,7 +2087,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>197</v>
@@ -1826,7 +2096,7 @@
         <v>198</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -1840,7 +2110,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>197</v>
@@ -1849,12 +2119,12 @@
         <v>199</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
@@ -1875,7 +2145,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
@@ -1892,7 +2162,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
@@ -1939,7 +2209,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>201</v>
@@ -1960,7 +2230,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>204</v>
@@ -1981,7 +2251,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>201</v>
@@ -2002,7 +2272,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>201</v>
@@ -2023,7 +2293,7 @@
         <v>28</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>204</v>
@@ -2044,7 +2314,7 @@
         <v>30</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>197</v>
@@ -2053,7 +2323,7 @@
         <v>209</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -2067,7 +2337,7 @@
         <v>32</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>197</v>
@@ -2088,7 +2358,7 @@
         <v>34</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>197</v>
@@ -2109,13 +2379,13 @@
         <v>36</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>197</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -2130,13 +2400,13 @@
         <v>38</v>
       </c>
       <c r="D19" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>249</v>
-      </c>
       <c r="F19" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -2150,13 +2420,13 @@
         <v>40</v>
       </c>
       <c r="D20" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>249</v>
-      </c>
       <c r="F20" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -2170,10 +2440,10 @@
         <v>42</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>248</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>249</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>203</v>
@@ -2190,13 +2460,13 @@
         <v>44</v>
       </c>
       <c r="D22" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>249</v>
-      </c>
       <c r="F22" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -2210,13 +2480,13 @@
         <v>46</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>249</v>
-      </c>
       <c r="F23" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -2230,13 +2500,13 @@
         <v>48</v>
       </c>
       <c r="D24" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="F24" s="8" t="s">
         <v>249</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -2256,7 +2526,7 @@
         <v>194</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2270,7 +2540,7 @@
         <v>52</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>204</v>
@@ -2290,7 +2560,7 @@
         <v>54</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>197</v>
@@ -2320,7 +2590,7 @@
         <v>214</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -2334,7 +2604,7 @@
         <v>58</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>204</v>
@@ -2354,13 +2624,13 @@
         <v>60</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -2374,13 +2644,13 @@
         <v>193</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -2394,13 +2664,13 @@
         <v>63</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -2414,13 +2684,13 @@
         <v>65</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E33" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="F33" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>219</v>
       </c>
       <c r="G33" s="3"/>
     </row>
@@ -2435,13 +2705,13 @@
         <v>67</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G34" s="3"/>
     </row>
@@ -2456,13 +2726,13 @@
         <v>69</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -2476,13 +2746,13 @@
         <v>71</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G36" s="3"/>
     </row>
@@ -2497,13 +2767,13 @@
         <v>73</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G37" s="3"/>
     </row>
@@ -2518,10 +2788,10 @@
         <v>75</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>203</v>
@@ -2539,13 +2809,13 @@
         <v>77</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -2559,13 +2829,13 @@
         <v>79</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G40" s="3"/>
     </row>
@@ -2580,13 +2850,13 @@
         <v>81</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G41" s="3"/>
     </row>
@@ -2601,220 +2871,220 @@
         <v>83</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="E43" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="E43" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="F43" s="29" t="s">
-        <v>225</v>
+      <c r="F43" s="30" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
+      <c r="A44" s="31"/>
+      <c r="B44" s="31"/>
       <c r="C44" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="30"/>
     </row>
     <row r="45" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D45" s="28" t="s">
+      <c r="D45" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="E45" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="E45" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="F45" s="29" t="s">
-        <v>227</v>
+      <c r="F45" s="30" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
+      <c r="A46" s="31"/>
+      <c r="B46" s="31"/>
       <c r="C46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="30"/>
     </row>
     <row r="47" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D47" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="E47" s="30" t="s">
         <v>255</v>
-      </c>
-      <c r="E47" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F47" s="11" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
+      <c r="A48" s="31"/>
+      <c r="B48" s="31"/>
       <c r="C48" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
       <c r="F48" s="11"/>
     </row>
     <row r="49" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A49" s="30" t="s">
+      <c r="A49" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D49" s="28" t="s">
+      <c r="D49" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="E49" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="E49" s="28" t="s">
-        <v>247</v>
-      </c>
       <c r="F49" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="30"/>
-      <c r="B50" s="30"/>
+      <c r="A50" s="31"/>
+      <c r="B50" s="31"/>
       <c r="C50" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
     </row>
     <row r="51" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A51" s="30" t="s">
+      <c r="A51" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="30" t="s">
+      <c r="B51" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="28" t="s">
+      <c r="D51" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="E51" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="E51" s="28" t="s">
-        <v>247</v>
-      </c>
       <c r="F51" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="30"/>
-      <c r="B52" s="30"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="31"/>
       <c r="C52" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
     </row>
     <row r="53" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A53" s="30" t="s">
+      <c r="A53" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D53" s="28" t="s">
+      <c r="D53" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="E53" s="29" t="s">
         <v>246</v>
-      </c>
-      <c r="E53" s="28" t="s">
-        <v>247</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="31"/>
       <c r="C54" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
     </row>
     <row r="55" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A55" s="30" t="s">
+      <c r="A55" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D55" s="28" t="s">
+      <c r="D55" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="E55" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="E55" s="28" t="s">
-        <v>247</v>
-      </c>
       <c r="F55" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
@@ -2827,13 +3097,13 @@
         <v>106</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E57" s="10" t="s">
         <v>197</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G57" s="3"/>
     </row>
@@ -2848,13 +3118,13 @@
         <v>108</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E58" s="10" t="s">
         <v>197</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G58" s="3"/>
     </row>
@@ -2872,10 +3142,10 @@
         <v>191</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -2895,7 +3165,7 @@
         <v>194</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G60" s="3"/>
     </row>
@@ -2916,7 +3186,7 @@
         <v>194</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G61" s="3"/>
     </row>
@@ -2937,7 +3207,7 @@
         <v>194</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G62" s="3"/>
     </row>
@@ -2952,13 +3222,13 @@
         <v>119</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E63" s="10" t="s">
         <v>197</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G63" s="3"/>
     </row>
@@ -2973,13 +3243,13 @@
         <v>121</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G64" s="3"/>
     </row>
@@ -2994,13 +3264,13 @@
         <v>123</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G65" s="3"/>
     </row>
@@ -3015,13 +3285,13 @@
         <v>125</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E66" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="F66" s="9" t="s">
         <v>234</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>235</v>
       </c>
       <c r="G66" s="3"/>
     </row>
@@ -3036,13 +3306,13 @@
         <v>127</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G67" s="3"/>
     </row>
@@ -3057,10 +3327,10 @@
         <v>129</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F68" s="9" t="s">
         <v>203</v>
@@ -3078,13 +3348,13 @@
         <v>131</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G69" s="3"/>
     </row>
@@ -3099,13 +3369,13 @@
         <v>133</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G70" s="3"/>
     </row>
@@ -3120,13 +3390,13 @@
         <v>135</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G71" s="3"/>
     </row>
@@ -3141,13 +3411,13 @@
         <v>137</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G72" s="3"/>
     </row>
@@ -3162,10 +3432,10 @@
         <v>139</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>203</v>
@@ -3183,13 +3453,13 @@
         <v>141</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G74" s="3"/>
     </row>
@@ -3204,13 +3474,13 @@
         <v>143</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G75" s="3"/>
     </row>
@@ -3225,13 +3495,13 @@
         <v>145</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G76" s="3"/>
     </row>
@@ -3246,13 +3516,13 @@
         <v>147</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G77" s="3"/>
     </row>
@@ -3267,10 +3537,10 @@
         <v>149</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F78" s="9" t="s">
         <v>203</v>
@@ -3333,7 +3603,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1E071C-8572-48FD-94ED-9BC2BF0CD944}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
@@ -3341,23 +3611,24 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E55" sqref="E55"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="1">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="1">
+      <selection activeCell="H2" sqref="H2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="73.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="77.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="73.5703125" style="4" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="61.85546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="49.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="44" style="4" customWidth="1"/>
-    <col min="7" max="7" width="69.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="7" max="8" width="62.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="65.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>154</v>
       </c>
@@ -3368,19 +3639,22 @@
         <v>20</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>205</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>155</v>
       </c>
@@ -3388,41 +3662,55 @@
         <v>156</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>388</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="I2" s="4" t="str">
+        <f>_xlfn.CONCAT("[",F2,"]","(",G2,")")</f>
+        <v>[date](StructureDefinition-eicr-composition-definitions.html#Composition.date)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>156</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="I3" s="4" t="str">
+        <f>_xlfn.CONCAT("[",F3,"]","(",G3,")")</f>
+        <v>[id](StructureDefinition-eicr-composition-definitions.html#Composition.id)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>96</v>
       </c>
@@ -3430,19 +3718,29 @@
         <v>157</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>261</v>
+        <v>395</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="I4" s="4" t="str">
+        <f>_xlfn.CONCAT("[",F4,"]","(",G4,")")</f>
+        <v>[identifier](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.identifier)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>99</v>
       </c>
@@ -3450,22 +3748,29 @@
         <v>157</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>375</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>261</v>
+        <v>373</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>395</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>203</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="I5" s="4" t="str">
+        <f t="shared" ref="I5:I56" si="0">_xlfn.CONCAT("[",F5,"]","(",G5,")")</f>
+        <v>[name](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.name)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>102</v>
       </c>
@@ -3473,19 +3778,29 @@
         <v>157</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>261</v>
+        <v>372</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>395</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="I6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[telecom[system="phone"]](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.telecom)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>93</v>
       </c>
@@ -3493,19 +3808,29 @@
         <v>157</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>261</v>
+        <v>371</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>395</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="I7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[telecom[system="fax"]](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.telecom)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>87</v>
       </c>
@@ -3513,19 +3838,29 @@
         <v>157</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>261</v>
+        <v>370</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>395</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="I8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[telecom[system="email"]](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.telecom)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>90</v>
       </c>
@@ -3533,19 +3868,29 @@
         <v>157</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="G9" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="I9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[name](StructureDefinition-eicr-location-definitions.html#Location.name)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>84</v>
       </c>
@@ -3553,19 +3898,29 @@
         <v>157</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="I10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[address](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.address)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -3573,19 +3928,29 @@
         <v>157</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="I11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[identifier](StructureDefinition-eicr-location-definitions.html#Location.identifier)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -3593,19 +3958,29 @@
         <v>157</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="I12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[name](StructureDefinition-eicr-location-definitions.html#Location.name)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
@@ -3613,19 +3988,29 @@
         <v>157</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="I13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[type](StructureDefinition-eicr-location-definitions.html#Location.type)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
@@ -3633,19 +4018,29 @@
         <v>157</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="I14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[telecom[system="phone"]](StructureDefinition-eicr-location-definitions.html#Location.telecom)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>158</v>
       </c>
@@ -3653,19 +4048,29 @@
         <v>157</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="I15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[telecom[system="fax"]](StructureDefinition-eicr-location-definitions.html#Location.telecom)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
@@ -3673,19 +4078,29 @@
         <v>157</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="I16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[address](StructureDefinition-eicr-location-definitions.html#Location.address)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
@@ -3696,16 +4111,26 @@
         <v>73</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="I17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[identifier](StructureDefinition-ecr-patient-definitions.html#Patient.identifier)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
@@ -3716,16 +4141,26 @@
         <v>75</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="I18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[name](StructureDefinition-ecr-patient-definitions.html#Patient.name)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>76</v>
       </c>
@@ -3736,16 +4171,26 @@
         <v>77</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="I19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[telecom[system="phone"]](StructureDefinition-ecr-patient-definitions.html#Patient.telecom)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
@@ -3756,16 +4201,26 @@
         <v>69</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="I20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[telecom[system="email"]](StructureDefinition-ecr-patient-definitions.html#Patient.telecom)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>61</v>
       </c>
@@ -3776,16 +4231,26 @@
         <v>193</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>218</v>
+        <v>257</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>400</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="I21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[contact.name](StructureDefinition-ecr-patient-definitions.html#Patient.contact.name)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>62</v>
       </c>
@@ -3796,16 +4261,26 @@
         <v>63</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>218</v>
+        <v>257</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>400</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="I22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[contact.telecom[system="phone"]](StructureDefinition-ecr-patient-definitions.html#Patient.contact.telecom)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>59</v>
       </c>
@@ -3816,16 +4291,26 @@
         <v>60</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>218</v>
+        <v>257</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>400</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="I23" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[contact.telecom[system="email"]](StructureDefinition-ecr-patient-definitions.html#Patient.contact.telecom)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>82</v>
       </c>
@@ -3836,16 +4321,26 @@
         <v>83</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>218</v>
+        <v>257</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>400</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="I24" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[address](StructureDefinition-ecr-patient-definitions.html#Patient.address)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>66</v>
       </c>
@@ -3856,36 +4351,56 @@
         <v>67</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>218</v>
+        <v>257</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>400</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="I25" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[birthdate](StructureDefinition-ecr-patient-definitions.html#Patient.birthdate)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>159</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="G26" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="I26" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[us-core-birthsex](StructureDefinition-ecr-patient-definitions.html#Patient.extension:birthsex)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>80</v>
       </c>
@@ -3896,16 +4411,26 @@
         <v>81</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>218</v>
+        <v>257</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>400</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="I27" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[us-core-race](StructureDefinition-ecr-patient-definitions.html#Patient.extension:race)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>70</v>
       </c>
@@ -3916,16 +4441,26 @@
         <v>71</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>218</v>
+        <v>257</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>400</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="I28" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[us-core-ethnicity](StructureDefinition-ecr-patient-definitions.html#Patient.extension:ethnicity)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>160</v>
       </c>
@@ -3936,59 +4471,86 @@
         <v>79</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>218</v>
+        <v>257</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>400</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="I29" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[communication.language](StructureDefinition-ecr-patient-definitions.html#Patient.communication.language)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>161</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="I30" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[valueCodeableConcept](StructureDefinition-eicr-occupationhistory-definitions.html#Observation)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>206</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="I31" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[valueCodeableConcept](StructureDefinition-pregnancy-status-definitions.html#Observation)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>164</v>
       </c>
@@ -3999,16 +4561,26 @@
         <v>48</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="I32" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[type](StructureDefinition-eicr-location-definitions.html#Location.type)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>165</v>
       </c>
@@ -4016,19 +4588,29 @@
         <v>157</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="I33" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[period.start](StructureDefinition-eicr-encounter-definitions.html#Encounter.period)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>166</v>
       </c>
@@ -4036,19 +4618,29 @@
         <v>157</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E34" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="F34" s="4" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="I34" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[period.start](StructureDefinition-eicr-encounter-definitions.html#Encounter.period)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>167</v>
       </c>
@@ -4056,19 +4648,29 @@
         <v>157</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="I35" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[period.end](StructureDefinition-eicr-encounter-definitions.html#Encounter.period)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>168</v>
       </c>
@@ -4076,16 +4678,26 @@
         <v>169</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="I36" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[text](StructureDefinition-eicr-composition-definitions.html#Composition.section:sliceHistoryOfPresentIllnessSection.text)</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>170</v>
       </c>
@@ -4093,230 +4705,350 @@
         <v>171</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="I37" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[text](StructureDefinition-eicr-composition-definitions.html#Composition.section:sliceReasonForVisitSection.text)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="I38" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[onset.start](StructureDefinition-eicr-condition-definitions.html#Condition.onset[x])</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>173</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="I39" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[code](StructureDefinition-eicr-condition-definitions.html#Condition.code)</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>174</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="I40" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[code](StructureDefinition-eicr-procedurerequest-definitions.html#ProcedureRequest.code)</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
         <v>175</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C41" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="C41" s="14" t="s">
-        <v>344</v>
-      </c>
       <c r="E41" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="I41" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[extension-eicr-trigger-code-flag](StructureDefinition-eicr-composition-definitions.html#Composition.section:slicePlanOfTreatmentSection.entry:sliceEICRProcedureRequest.extension:sliceTriggerEICRProcedureRequest)</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+        <v>333</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="I42" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[code and/or valueCodeableConcept](https://www.hl7.org/fhir/us/core/StructureDefinition-us-core-observationresults-definitions.html#Observation.code)</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>177</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="I43" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[extension-eicr-trigger-code-flag](StructureDefinition-eicr-composition-definitions.html#Composition.section:sliceResultsSection.entry:sliceUSCoreObservationResults.extension:sliceTriggerUSCoreObservationResults)</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>178</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="I44" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[identifier](StructureDefinition-us-core-observationresults-definitions.html#Observation.identifier)</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>179</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>163</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="I45" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[code](StructureDefinition-eicr-condition-definitions.html#Condition.code)</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>181</v>
       </c>
       <c r="D46" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="E46" s="4" t="s">
-        <v>328</v>
-      </c>
       <c r="F46" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="I46" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[extension-eicr-trigger-code-flag](StructureDefinition-eicr-composition-definitions.html#Composition.section:sliceProblemSection.entry:sliceEICRCondition.extension:sliceTriggerCondition)</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>163</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="I47" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[assertedDate](StructureDefinition-eicr-condition-definitions.html#Condition.assertedDate)</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>183</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>184</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="I48" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[medication[x]](https://www.hl7.org/fhir/us/core/StructureDefinition-us-core-medicationstatement-definitions.html#MedicationStatement.medication[x])</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>185</v>
       </c>
@@ -4324,119 +5056,176 @@
         <v>157</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>218</v>
+        <v>400</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>319</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="I49" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[deceasedDateTime](StructureDefinition-ecr-patient-definitions.html#Patient.deceased[x])</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+        <v>335</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="I50" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[](https://www.hl7.org/fhir/us/core/StructureDefinition-us-core-immunization.html)</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="I51" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[effective[x]](StructureDefinition-eicr-travel-history-definitions.html#Observation.effective[x])</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>351</v>
       </c>
-      <c r="C52" s="14" t="s">
-        <v>353</v>
-      </c>
       <c r="D52" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E52" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="F52" s="4" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G52" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="I52" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[component.valueCodeableConcept.text](StructureDefinition-eicr-travel-history-definitions.html#Observation.component.valueCodeableConcept:valueCodeableConcept.text)</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="I53" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[component.valueCodeableConcept.coding](StructureDefinition-eicr-travel-history-definitions.html#Observation.component.valueCodeableConcept:valueCodeableConcept.coding)</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="I54" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[component.valueCodeableConcept.coding.extension-eicr-travel-history-address](StructureDefinition-eicr-travel-history-definitions.html#Observation.component.valueCodeableConcept:valueCodeableConcept.extension:travelHistoryAddress)</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>55</v>
       </c>
@@ -4444,33 +5233,50 @@
         <v>157</v>
       </c>
       <c r="C55" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="I55" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[extension-eicr-manually-initiated-reason](StructureDefinition-eicr-composition-definitions.html#Composition.extension:extensionEICRManuallyInitiatedReason)</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E56" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="F55" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>379</v>
+      <c r="G56" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="I56" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>[extension-eicr-manually-initiated-reason.valueString](StructureDefinition-eicr-composition-definitions.html#Composition.extension:extensionEICRManuallyInitiatedReason)</v>
       </c>
     </row>
   </sheetData>
@@ -4490,421 +5296,421 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="29.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="24" t="s">
+      <c r="B4" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>288</v>
       </c>
-      <c r="D2" s="21"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="D11" s="22"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="24" t="s">
         <v>279</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="C12" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="22"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="D17" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>289</v>
-      </c>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>280</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>293</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="D4" s="21"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="D5" s="21" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="D20" s="22"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="D21" s="22"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="D22" s="22"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="D23" s="22"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="D24" s="22"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="D25" s="22"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="D26" s="22"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="24" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="D6" s="21"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="D7" s="21"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="D9" s="21"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>281</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="21"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>286</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>287</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>284</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>284</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>284</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="D16" s="21"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="D17" s="21" t="s">
+      <c r="C27" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="D27" s="22"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="C28" s="28" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="D18" s="21"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="D20" s="21"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="D21" s="21"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="D22" s="21"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="D23" s="21"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="D24" s="21"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="D25" s="21"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="D26" s="21"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="23" t="s">
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="24" t="s">
         <v>297</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C29" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="D29" s="22"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>303</v>
+      </c>
+      <c r="D30" s="22"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="D31" s="22"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="C32" s="28" t="s">
         <v>304</v>
       </c>
-      <c r="D27" s="21"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>298</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="D28" s="21"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>299</v>
-      </c>
-      <c r="C29" s="27" t="s">
+      <c r="D32" s="22"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="C33" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="D29" s="21"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>305</v>
-      </c>
-      <c r="D30" s="21"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>301</v>
-      </c>
-      <c r="C31" s="27" t="s">
-        <v>308</v>
-      </c>
-      <c r="D31" s="21"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>300</v>
-      </c>
-      <c r="C32" s="27" t="s">
-        <v>306</v>
-      </c>
-      <c r="D32" s="21"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>303</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>309</v>
-      </c>
-      <c r="D33" s="21"/>
+      <c r="D33" s="22"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C34" s="18"/>
+      <c r="C34" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5142,19 +5948,19 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B0C849C-1E0C-4B3D-9203-5FFDB8062BA1}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="6FDAA894-E433-443A-929C-6668B5175CA9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="6fdaa894-e433-443a-929c-6668b5175ca9"/>
     <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
+    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6FDAA894-E433-443A-929C-6668B5175CA9"/>
-    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Error fixes, remove old files etc.
</commit_message>
<xml_diff>
--- a/mapping/Mappings.xlsx
+++ b/mapping/Mappings.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Documents\Work\SourceControl\GitHub\FHIR\case-reporting\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D3DDD7-222C-4788-98EB-50E683F715F5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93634875-B76F-4144-98DE-D769FAB20C9C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="7665" activeTab="1" xr2:uid="{69CB834B-E9B6-4361-B34A-B68FB7F004FE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9120" activeTab="1" xr2:uid="{5841EBE6-5BE3-4CB9-848A-445F7155F330}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="7665" xr2:uid="{69CB834B-E9B6-4361-B34A-B68FB7F004FE}"/>
   </bookViews>
   <sheets>
     <sheet name="RR" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="502">
   <si>
     <t>Date and time of eICR Receipt</t>
   </si>
@@ -1192,15 +1192,6 @@
     <t>ID of the eICR Document</t>
   </si>
   <si>
-    <t>StructureDefinition-extension-rr-determination-of-reportability-reason.html</t>
-  </si>
-  <si>
-    <t>StructureDefinition-extension-rr-determination-of-reportability-rule.html</t>
-  </si>
-  <si>
-    <t>StructureDefinition-extension-rr-determination-of-reportability.html</t>
-  </si>
-  <si>
     <t>StructureDefinition-extension-rr-external-resource-type.html</t>
   </si>
   <si>
@@ -1496,6 +1487,66 @@
   </si>
   <si>
     <t>[identifier](http://hl7.org/fhir/us/core/StructureDefinition-us-core-practitioner-definitions.html#Practitioner.identifier)</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-relevant-reportable-condition-plandefinition-definitions.html#PlanDefinition.extension:determinationOfReportabilityReason</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-relevant-reportable-condition-plandefinition-definitions.html#PlanDefinition.extension:determinationOfReportabilityRule</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-relevant-reportable-condition-plandefinition-definitions.html#PlanDefinition.extension:determinationOfReportability</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-communication-definitions.html#Communication.payload:sliceEICRInformation.extension:extensionEICRReceiptTime</t>
+  </si>
+  <si>
+    <t>extension-rr-eicr-receipt-time</t>
+  </si>
+  <si>
+    <t>Communication[rr-communication].payload.extension</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-communication-definitions.html#Communication.payload:sliceEICRInformation.contentReference:contentReference.identifier</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-communication-definitions.html#Communication.context</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.gender</t>
+  </si>
+  <si>
+    <t>Communication.payload:sliceEICRInformation.extension:eICRProcessingStatus</t>
+  </si>
+  <si>
+    <t>StructureDefinition-extension-rr-eicr-processing-status-definitions.html#Extension.extension:eICRValidationOutput.value[x]</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-eicr-processing-status-reason-definitions.html#Observation.valueCodeableConcept:valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-relevant-reportable-condition-plandefinition-definitions.html#PlanDefinition.action.documentation.display</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-relevant-reportable-condition-plandefinition-definitions.html#PlanDefinition.action.documentation.url</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-relevant-reportable-condition-plandefinition-definitions.html#PlanDefinition.action.documentation.extension:externalResourcePriority</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-communication-definitions.html#Communication.payload:sliceEICRInformation.contentReference:contentReference.display</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-eicr-processing-status-reason-definitions.html#Observation.component.value[x]</t>
+  </si>
+  <si>
+    <t>StructureDefinition-rr-relevant-reportable-condition-plandefinition-definitions.html#PlanDefinition.jurisdiction.extension:locationRelevance</t>
+  </si>
+  <si>
+    <t>birthDate</t>
+  </si>
+  <si>
+    <t>StructureDefinition-ecr-patient-definitions.html#Patient.birthDate</t>
   </si>
 </sst>
 </file>
@@ -1602,7 +1653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1642,6 +1693,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1995,25 +2049,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2E64F1-05B1-4B7F-9A17-F737E551CA1E}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
-    <sheetView topLeftCell="D1" workbookViewId="1">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane xSplit="1" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="77.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="33.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="77.140625" style="4"/>
     <col min="4" max="4" width="36.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="106.5703125" style="5" customWidth="1"/>
     <col min="8" max="16384" width="77.140625" style="4"/>
   </cols>
   <sheetData>
@@ -2040,7 +2097,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2050,8 +2107,15 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="16" t="s">
+        <v>487</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -2073,7 +2137,7 @@
         <v>196</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>383</v>
+        <v>482</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="36" x14ac:dyDescent="0.2">
@@ -2096,7 +2160,7 @@
         <v>198</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>384</v>
+        <v>483</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -2119,10 +2183,10 @@
         <v>199</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>264</v>
       </c>
@@ -2141,7 +2205,9 @@
       <c r="F6" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -2196,7 +2262,9 @@
       <c r="F9" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -2217,7 +2285,9 @@
       <c r="F10" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -2259,9 +2329,11 @@
       <c r="F12" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12" s="3" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -2280,7 +2352,9 @@
       <c r="F13" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -2301,9 +2375,11 @@
       <c r="F14" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="G14" s="3" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
@@ -2323,7 +2399,7 @@
         <v>209</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -2345,7 +2421,9 @@
       <c r="F16" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -2366,9 +2444,11 @@
       <c r="F17" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="3" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -2387,7 +2467,9 @@
       <c r="F18" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -2408,6 +2490,9 @@
       <c r="F19" s="8" t="s">
         <v>224</v>
       </c>
+      <c r="G19" s="5" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -2428,6 +2513,9 @@
       <c r="F20" s="8" t="s">
         <v>221</v>
       </c>
+      <c r="G20" s="5" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -2448,6 +2536,9 @@
       <c r="F21" s="8" t="s">
         <v>203</v>
       </c>
+      <c r="G21" s="5" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -2468,6 +2559,9 @@
       <c r="F22" s="8" t="s">
         <v>250</v>
       </c>
+      <c r="G22" s="5" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -2488,6 +2582,9 @@
       <c r="F23" s="8" t="s">
         <v>225</v>
       </c>
+      <c r="G23" s="5" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -2508,8 +2605,11 @@
       <c r="F24" s="8" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
@@ -2527,6 +2627,9 @@
       </c>
       <c r="F25" s="13" t="s">
         <v>267</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2548,6 +2651,9 @@
       <c r="F26" s="9" t="s">
         <v>216</v>
       </c>
+      <c r="G26" s="3" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -2568,9 +2674,11 @@
       <c r="F27" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+      <c r="G27" s="3" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
@@ -2590,7 +2698,7 @@
         <v>214</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -2612,6 +2720,9 @@
       <c r="F29" s="9" t="s">
         <v>217</v>
       </c>
+      <c r="G29" s="3" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
@@ -2627,10 +2738,13 @@
         <v>240</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>251</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -2647,10 +2761,13 @@
         <v>240</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>252</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -2667,10 +2784,13 @@
         <v>240</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>253</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -2687,12 +2807,14 @@
         <v>240</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="G33" s="3"/>
+      <c r="G33" s="3" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
@@ -2708,12 +2830,14 @@
         <v>240</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="G34" s="3"/>
+        <v>500</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
@@ -2729,10 +2853,13 @@
         <v>240</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>226</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -2749,7 +2876,7 @@
         <v>240</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>220</v>
@@ -2770,7 +2897,7 @@
         <v>240</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>221</v>
@@ -2791,7 +2918,7 @@
         <v>240</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>203</v>
@@ -2812,7 +2939,7 @@
         <v>240</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>225</v>
@@ -2832,7 +2959,7 @@
         <v>240</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>222</v>
@@ -2853,7 +2980,7 @@
         <v>240</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>223</v>
@@ -2874,86 +3001,86 @@
         <v>240</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="29" t="s">
+      <c r="D43" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="E43" s="29" t="s">
+      <c r="E43" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="F43" s="30" t="s">
+      <c r="F43" s="31" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="32"/>
       <c r="C44" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="31"/>
     </row>
     <row r="45" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D45" s="29" t="s">
+      <c r="D45" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="E45" s="29" t="s">
+      <c r="E45" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="F45" s="30" t="s">
+      <c r="F45" s="31" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
+      <c r="A46" s="32"/>
+      <c r="B46" s="32"/>
       <c r="C46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="31"/>
     </row>
     <row r="47" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="30" t="s">
+      <c r="D47" s="31" t="s">
         <v>254</v>
       </c>
-      <c r="E47" s="30" t="s">
+      <c r="E47" s="31" t="s">
         <v>255</v>
       </c>
       <c r="F47" s="11" t="s">
@@ -2961,29 +3088,29 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="32"/>
       <c r="C48" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
       <c r="F48" s="11"/>
     </row>
     <row r="49" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D49" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="E49" s="29" t="s">
+      <c r="E49" s="30" t="s">
         <v>246</v>
       </c>
       <c r="F49" s="8" t="s">
@@ -2991,28 +3118,28 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
+      <c r="A50" s="32"/>
+      <c r="B50" s="32"/>
       <c r="C50" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
     </row>
     <row r="51" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="D51" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="E51" s="29" t="s">
+      <c r="E51" s="30" t="s">
         <v>246</v>
       </c>
       <c r="F51" s="8" t="s">
@@ -3020,28 +3147,28 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="31"/>
-      <c r="B52" s="31"/>
+      <c r="A52" s="32"/>
+      <c r="B52" s="32"/>
       <c r="C52" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
     </row>
     <row r="53" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A53" s="31" t="s">
+      <c r="A53" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="B53" s="31" t="s">
+      <c r="B53" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D53" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="E53" s="29" t="s">
+      <c r="E53" s="30" t="s">
         <v>246</v>
       </c>
       <c r="F53" s="8" t="s">
@@ -3049,28 +3176,28 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A54" s="31"/>
-      <c r="B54" s="31"/>
+      <c r="A54" s="32"/>
+      <c r="B54" s="32"/>
       <c r="C54" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
     </row>
     <row r="55" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="31" t="s">
+      <c r="B55" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D55" s="29" t="s">
+      <c r="D55" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="E55" s="29" t="s">
+      <c r="E55" s="30" t="s">
         <v>246</v>
       </c>
       <c r="F55" s="8" t="s">
@@ -3078,15 +3205,15 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="31"/>
-      <c r="B56" s="31"/>
+      <c r="A56" s="32"/>
+      <c r="B56" s="32"/>
       <c r="C56" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D56" s="29"/>
-      <c r="E56" s="29"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+    </row>
+    <row r="57" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>105</v>
       </c>
@@ -3107,7 +3234,7 @@
       </c>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>107</v>
       </c>
@@ -3190,7 +3317,7 @@
       </c>
       <c r="G61" s="3"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>116</v>
       </c>
@@ -3605,14 +3732,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1E071C-8572-48FD-94ED-9BC2BF0CD944}">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E55" sqref="E55"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="1">
-      <selection activeCell="H2" sqref="H2:H4"/>
+    <sheetView topLeftCell="F1" workbookViewId="1">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3672,10 +3799,10 @@
         <v>259</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="I2" s="4" t="str">
         <f>_xlfn.CONCAT("[",F2,"]","(",G2,")")</f>
@@ -3700,10 +3827,10 @@
         <v>380</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="I3" s="4" t="str">
         <f>_xlfn.CONCAT("[",F3,"]","(",G3,")")</f>
@@ -3721,7 +3848,7 @@
         <v>374</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>246</v>
@@ -3730,10 +3857,10 @@
         <v>221</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="I4" s="4" t="str">
         <f>_xlfn.CONCAT("[",F4,"]","(",G4,")")</f>
@@ -3751,7 +3878,7 @@
         <v>373</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>246</v>
@@ -3760,10 +3887,10 @@
         <v>203</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="I5" s="4" t="str">
         <f t="shared" ref="I5:I56" si="0">_xlfn.CONCAT("[",F5,"]","(",G5,")")</f>
@@ -3781,7 +3908,7 @@
         <v>372</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>246</v>
@@ -3790,10 +3917,10 @@
         <v>225</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="I6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3811,7 +3938,7 @@
         <v>371</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>246</v>
@@ -3820,10 +3947,10 @@
         <v>250</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="I7" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3841,7 +3968,7 @@
         <v>370</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>246</v>
@@ -3850,10 +3977,10 @@
         <v>226</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I8" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3880,10 +4007,10 @@
         <v>203</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3910,10 +4037,10 @@
         <v>224</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="I10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3940,10 +4067,10 @@
         <v>221</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="I11" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3970,10 +4097,10 @@
         <v>203</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I12" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4000,10 +4127,10 @@
         <v>249</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="I13" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4030,10 +4157,10 @@
         <v>225</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="I14" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4060,10 +4187,10 @@
         <v>250</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="I15" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4090,10 +4217,10 @@
         <v>224</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="I16" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4114,16 +4241,16 @@
         <v>257</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>221</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="I17" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4144,16 +4271,16 @@
         <v>257</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>203</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="I18" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4174,16 +4301,16 @@
         <v>257</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>225</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="I19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4204,16 +4331,16 @@
         <v>257</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>226</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="I20" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4234,16 +4361,16 @@
         <v>257</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>252</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="I21" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4264,16 +4391,16 @@
         <v>257</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>253</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="I22" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4294,16 +4421,16 @@
         <v>257</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>251</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="I23" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4324,16 +4451,16 @@
         <v>257</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>224</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="I24" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4354,16 +4481,16 @@
         <v>257</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>219</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="I25" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4384,16 +4511,16 @@
         <v>257</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>258</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="I26" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4414,16 +4541,16 @@
         <v>257</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>223</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="I27" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4444,16 +4571,16 @@
         <v>257</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>220</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="I28" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4474,16 +4601,16 @@
         <v>257</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>222</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="I29" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4510,10 +4637,10 @@
         <v>206</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="I30" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4540,10 +4667,10 @@
         <v>206</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="I31" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4570,10 +4697,10 @@
         <v>249</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="I32" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4600,10 +4727,10 @@
         <v>310</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="I33" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4630,10 +4757,10 @@
         <v>310</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="I34" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4660,10 +4787,10 @@
         <v>311</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="I35" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4687,10 +4814,10 @@
         <v>234</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="I36" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4714,10 +4841,10 @@
         <v>234</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="I37" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4744,10 +4871,10 @@
         <v>313</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="I38" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4774,10 +4901,10 @@
         <v>202</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="I39" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4804,10 +4931,10 @@
         <v>202</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="I40" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4831,10 +4958,10 @@
         <v>323</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="I41" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4861,10 +4988,10 @@
         <v>333</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="I42" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4888,10 +5015,10 @@
         <v>323</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I43" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4918,10 +5045,10 @@
         <v>221</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="I44" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4948,10 +5075,10 @@
         <v>202</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="I45" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4978,10 +5105,10 @@
         <v>323</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="I46" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5008,10 +5135,10 @@
         <v>329</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="I47" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5038,10 +5165,10 @@
         <v>331</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="I48" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5062,16 +5189,16 @@
         <v>257</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>319</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="I49" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5095,10 +5222,10 @@
         <v>335</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I50" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5125,10 +5252,10 @@
         <v>315</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I51" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5155,10 +5282,10 @@
         <v>316</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="I52" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5185,10 +5312,10 @@
         <v>317</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="I53" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5215,10 +5342,10 @@
         <v>318</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="I54" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5242,10 +5369,10 @@
         <v>376</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I55" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5269,10 +5396,10 @@
         <v>377</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="I56" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5296,421 +5423,421 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="29.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>276</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="26" t="s">
         <v>286</v>
       </c>
-      <c r="D2" s="22"/>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>277</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="26" t="s">
         <v>287</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>278</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="25" t="s">
         <v>291</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="26" t="s">
         <v>288</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>289</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="23" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="25" t="s">
         <v>289</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="25" t="s">
         <v>289</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="23"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="25" t="s">
         <v>289</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="23"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>289</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="23"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>289</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="23"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>289</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="D11" s="22"/>
+      <c r="D11" s="23"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="25" t="s">
         <v>279</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="23"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="29" t="s">
         <v>285</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="23" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="23" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="D15" s="22"/>
+      <c r="D15" s="23"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="23"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="23" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="23"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D19" s="22"/>
+      <c r="D19" s="23"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D20" s="22"/>
+      <c r="D20" s="23"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D21" s="22"/>
+      <c r="D21" s="23"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="23"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D23" s="22"/>
+      <c r="D23" s="23"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D24" s="22"/>
+      <c r="D24" s="23"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D25" s="22"/>
+      <c r="D25" s="23"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D26" s="22"/>
+      <c r="D26" s="23"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25" t="s">
         <v>295</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="29" t="s">
         <v>302</v>
       </c>
-      <c r="D27" s="22"/>
+      <c r="D27" s="23"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="25" t="s">
         <v>296</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="D28" s="22"/>
+      <c r="D28" s="23"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="25" t="s">
         <v>297</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="D29" s="22"/>
+      <c r="D29" s="23"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="25" t="s">
         <v>300</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="29" t="s">
         <v>303</v>
       </c>
-      <c r="D30" s="22"/>
+      <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="25" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="29" t="s">
         <v>306</v>
       </c>
-      <c r="D31" s="22"/>
+      <c r="D31" s="23"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="29" t="s">
         <v>304</v>
       </c>
-      <c r="D32" s="22"/>
+      <c r="D32" s="23"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="25" t="s">
         <v>301</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="29" t="s">
         <v>307</v>
       </c>
-      <c r="D33" s="22"/>
+      <c r="D33" s="23"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C34" s="19"/>
+      <c r="C34" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>